<commit_message>
Minor changes in scripts and formatting
</commit_message>
<xml_diff>
--- a/models/Master.xlsx
+++ b/models/Master.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-120" windowWidth="28800" windowHeight="11805" firstSheet="5" activeTab="11"/>
+    <workbookView xWindow="0" yWindow="-120" windowWidth="28800" windowHeight="11220" firstSheet="9" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="Beskrivning" sheetId="19" r:id="rId1"/>
@@ -6764,63 +6764,63 @@
     <xf numFmtId="0" fontId="26" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="21" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="26" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -6839,6 +6839,33 @@
     <xf numFmtId="0" fontId="22" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="26" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="22" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -6857,33 +6884,6 @@
     <xf numFmtId="0" fontId="22" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="19" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -6902,54 +6902,54 @@
     <xf numFmtId="0" fontId="22" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="21" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="3" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="3" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="26" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -6968,26 +6968,32 @@
     <xf numFmtId="0" fontId="22" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="76" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="78" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="74" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="60" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="72" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="76" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="78" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="62" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="71" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="74" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="79" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="73" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="60" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -6995,12 +7001,6 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="62" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="79" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="73" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -7031,23 +7031,23 @@
     <xf numFmtId="0" fontId="10" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="3" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="5" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="23" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="3" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="5" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="29">
@@ -12034,10 +12034,10 @@
   <sheetPr>
     <tabColor rgb="FFD70000"/>
   </sheetPr>
-  <dimension ref="A1:J26"/>
+  <dimension ref="A2:J27"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:I3"/>
+    <sheetView zoomScale="82" zoomScaleNormal="82" workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12047,146 +12047,142 @@
     <col min="3" max="16384" width="8.85546875" style="26"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="18" x14ac:dyDescent="0.25">
-      <c r="A1" s="117" t="s">
+    <row r="2" spans="1:10" ht="18" x14ac:dyDescent="0.25">
+      <c r="A2" s="117" t="s">
         <v>378</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="3" spans="1:10" ht="308.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="769" t="s">
+    <row r="3" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="1:10" ht="308.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="769" t="s">
         <v>376</v>
       </c>
-      <c r="B3" s="769"/>
-      <c r="C3" s="769"/>
-      <c r="D3" s="769"/>
-      <c r="E3" s="769"/>
-      <c r="F3" s="769"/>
-      <c r="G3" s="769"/>
-      <c r="H3" s="769"/>
-      <c r="I3" s="769"/>
-      <c r="J3" s="18"/>
-    </row>
-    <row r="4" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="5" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="105" t="s">
+      <c r="B4" s="769"/>
+      <c r="C4" s="769"/>
+      <c r="D4" s="769"/>
+      <c r="E4" s="769"/>
+      <c r="F4" s="769"/>
+      <c r="G4" s="769"/>
+      <c r="H4" s="769"/>
+      <c r="I4" s="769"/>
+      <c r="J4" s="18"/>
+    </row>
+    <row r="5" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="6" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="105" t="s">
         <v>244</v>
       </c>
-      <c r="B5" s="147" t="s">
+      <c r="B6" s="147" t="s">
         <v>67</v>
       </c>
-      <c r="C5" s="38"/>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="284" t="s">
+      <c r="C6" s="38"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="284" t="s">
         <v>177</v>
       </c>
-      <c r="B6" s="285" t="s">
+      <c r="B7" s="285" t="s">
         <v>277</v>
-      </c>
-      <c r="C6" s="38"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="286" t="s">
-        <v>339</v>
-      </c>
-      <c r="B7" s="287" t="s">
-        <v>340</v>
       </c>
       <c r="C7" s="38"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="286" t="s">
-        <v>278</v>
+        <v>339</v>
       </c>
       <c r="B8" s="287" t="s">
-        <v>276</v>
+        <v>340</v>
       </c>
       <c r="C8" s="38"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="286" t="s">
-        <v>367</v>
+        <v>278</v>
       </c>
       <c r="B9" s="287" t="s">
-        <v>368</v>
+        <v>276</v>
       </c>
       <c r="C9" s="38"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="286" t="s">
-        <v>241</v>
+        <v>367</v>
       </c>
       <c r="B10" s="287" t="s">
-        <v>208</v>
+        <v>368</v>
       </c>
       <c r="C10" s="38"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="286" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B11" s="287" t="s">
-        <v>245</v>
+        <v>208</v>
       </c>
       <c r="C11" s="38"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="286" t="s">
+        <v>242</v>
+      </c>
+      <c r="B12" s="287" t="s">
+        <v>245</v>
+      </c>
+      <c r="C12" s="38"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" s="286" t="s">
         <v>243</v>
       </c>
-      <c r="B12" s="287" t="s">
+      <c r="B13" s="287" t="s">
         <v>246</v>
       </c>
-      <c r="C12" s="38"/>
-    </row>
-    <row r="13" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="288" t="s">
+      <c r="C13" s="38"/>
+    </row>
+    <row r="14" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="288" t="s">
         <v>176</v>
       </c>
-      <c r="B13" s="289" t="s">
+      <c r="B14" s="289" t="s">
         <v>247</v>
       </c>
-      <c r="C13" s="38"/>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="361" t="s">
+      <c r="C14" s="38"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" s="361" t="s">
         <v>341</v>
-      </c>
-      <c r="B15" s="205"/>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="205" t="s">
-        <v>342</v>
       </c>
       <c r="B16" s="205"/>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="205" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="B17" s="205"/>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="205" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="B18" s="205"/>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="205" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="B19" s="205"/>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="205" t="s">
+        <v>345</v>
+      </c>
+      <c r="B20" s="205"/>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="205" t="s">
         <v>346</v>
       </c>
-      <c r="B20" s="205"/>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="205"/>
       <c r="B21" s="205"/>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
@@ -12209,9 +12205,13 @@
       <c r="A26" s="205"/>
       <c r="B26" s="205"/>
     </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="205"/>
+      <c r="B27" s="205"/>
+    </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A3:I3"/>
+    <mergeCell ref="A4:I4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -14247,7 +14247,7 @@
   </sheetPr>
   <dimension ref="A1:I277"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection activeCell="A6" sqref="A6"/>
       <selection pane="topRight" activeCell="A59" sqref="A59"/>
@@ -14264,28 +14264,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="842" t="s">
+      <c r="A1" s="840" t="s">
         <v>408</v>
       </c>
-      <c r="B1" s="846" t="s">
+      <c r="B1" s="842" t="s">
         <v>424</v>
       </c>
-      <c r="C1" s="846"/>
-      <c r="D1" s="846" t="s">
+      <c r="C1" s="842"/>
+      <c r="D1" s="842" t="s">
         <v>403</v>
       </c>
-      <c r="E1" s="846"/>
-      <c r="F1" s="846"/>
-      <c r="G1" s="846"/>
-      <c r="H1" s="840" t="s">
+      <c r="E1" s="842"/>
+      <c r="F1" s="842"/>
+      <c r="G1" s="842"/>
+      <c r="H1" s="843" t="s">
         <v>405</v>
       </c>
-      <c r="I1" s="844" t="s">
+      <c r="I1" s="845" t="s">
         <v>420</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="843"/>
+      <c r="A2" s="841"/>
       <c r="B2" s="593">
         <v>2030</v>
       </c>
@@ -14304,8 +14304,8 @@
       <c r="G2" s="593" t="s">
         <v>471</v>
       </c>
-      <c r="H2" s="841"/>
-      <c r="I2" s="845"/>
+      <c r="H2" s="844"/>
+      <c r="I2" s="846"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="594" t="s">
@@ -14592,20 +14592,20 @@
       <c r="A17" s="611" t="s">
         <v>423</v>
       </c>
-      <c r="B17" s="840" t="s">
+      <c r="B17" s="843" t="s">
         <v>424</v>
       </c>
-      <c r="C17" s="844"/>
-      <c r="D17" s="847" t="s">
+      <c r="C17" s="845"/>
+      <c r="D17" s="849" t="s">
         <v>403</v>
       </c>
-      <c r="E17" s="848"/>
+      <c r="E17" s="850"/>
       <c r="F17" s="612"/>
       <c r="G17" s="594"/>
-      <c r="H17" s="840" t="s">
+      <c r="H17" s="843" t="s">
         <v>405</v>
       </c>
-      <c r="I17" s="844" t="s">
+      <c r="I17" s="845" t="s">
         <v>420</v>
       </c>
     </row>
@@ -14625,8 +14625,8 @@
       </c>
       <c r="F18" s="592"/>
       <c r="G18" s="607"/>
-      <c r="H18" s="841"/>
-      <c r="I18" s="845"/>
+      <c r="H18" s="844"/>
+      <c r="I18" s="846"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="595" t="s">
@@ -14791,20 +14791,20 @@
       <c r="A30" s="611" t="s">
         <v>430</v>
       </c>
-      <c r="B30" s="847" t="s">
+      <c r="B30" s="849" t="s">
         <v>432</v>
       </c>
-      <c r="C30" s="848"/>
+      <c r="C30" s="850"/>
       <c r="D30" s="851" t="s">
         <v>431</v>
       </c>
       <c r="E30" s="852"/>
       <c r="F30" s="612"/>
       <c r="G30" s="594"/>
-      <c r="H30" s="840" t="s">
+      <c r="H30" s="843" t="s">
         <v>405</v>
       </c>
-      <c r="I30" s="844" t="s">
+      <c r="I30" s="845" t="s">
         <v>420</v>
       </c>
     </row>
@@ -14824,8 +14824,8 @@
       </c>
       <c r="F31" s="592"/>
       <c r="G31" s="607"/>
-      <c r="H31" s="841"/>
-      <c r="I31" s="845"/>
+      <c r="H31" s="844"/>
+      <c r="I31" s="846"/>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="595" t="s">
@@ -15443,20 +15443,20 @@
       <c r="A60" s="611" t="s">
         <v>511</v>
       </c>
-      <c r="B60" s="847" t="s">
+      <c r="B60" s="849" t="s">
         <v>424</v>
       </c>
-      <c r="C60" s="848"/>
-      <c r="D60" s="847" t="s">
+      <c r="C60" s="850"/>
+      <c r="D60" s="849" t="s">
         <v>403</v>
       </c>
       <c r="E60" s="853"/>
       <c r="F60" s="853"/>
-      <c r="G60" s="848"/>
-      <c r="H60" s="849" t="s">
+      <c r="G60" s="850"/>
+      <c r="H60" s="847" t="s">
         <v>405</v>
       </c>
-      <c r="I60" s="844" t="s">
+      <c r="I60" s="845" t="s">
         <v>420</v>
       </c>
     </row>
@@ -15480,8 +15480,8 @@
       <c r="G61" s="609" t="s">
         <v>471</v>
       </c>
-      <c r="H61" s="850"/>
-      <c r="I61" s="845"/>
+      <c r="H61" s="848"/>
+      <c r="I61" s="846"/>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62" s="595" t="s">
@@ -15888,23 +15888,23 @@
       <c r="I78" s="595"/>
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A79" s="842" t="s">
+      <c r="A79" s="840" t="s">
         <v>408</v>
       </c>
-      <c r="B79" s="846" t="s">
+      <c r="B79" s="842" t="s">
         <v>424</v>
       </c>
-      <c r="C79" s="846"/>
-      <c r="D79" s="846" t="s">
+      <c r="C79" s="842"/>
+      <c r="D79" s="842" t="s">
         <v>403</v>
       </c>
-      <c r="E79" s="846"/>
-      <c r="F79" s="846"/>
-      <c r="G79" s="846"/>
+      <c r="E79" s="842"/>
+      <c r="F79" s="842"/>
+      <c r="G79" s="842"/>
       <c r="I79" s="595"/>
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A80" s="843"/>
+      <c r="A80" s="841"/>
       <c r="B80" s="593">
         <v>2030</v>
       </c>
@@ -17505,6 +17505,15 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="H1:H2"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="I1:I2"/>
+    <mergeCell ref="H17:H18"/>
+    <mergeCell ref="I17:I18"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="D1:G1"/>
+    <mergeCell ref="D17:E17"/>
     <mergeCell ref="A79:A80"/>
     <mergeCell ref="B79:C79"/>
     <mergeCell ref="D79:G79"/>
@@ -17516,15 +17525,6 @@
     <mergeCell ref="D30:E30"/>
     <mergeCell ref="D60:G60"/>
     <mergeCell ref="B60:C60"/>
-    <mergeCell ref="H1:H2"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="I1:I2"/>
-    <mergeCell ref="H17:H18"/>
-    <mergeCell ref="I17:I18"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="D1:G1"/>
-    <mergeCell ref="D17:E17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -17538,7 +17538,7 @@
   </sheetPr>
   <dimension ref="A1:O27"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView topLeftCell="A2" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
@@ -17595,7 +17595,7 @@
       <c r="O3" s="118"/>
     </row>
     <row r="4" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="775" t="s">
+      <c r="A4" s="786" t="s">
         <v>289</v>
       </c>
       <c r="B4" s="859" t="s">
@@ -17757,7 +17757,7 @@
       <c r="O9" s="38"/>
     </row>
     <row r="10" spans="1:15" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="776"/>
+      <c r="A10" s="790"/>
       <c r="B10" s="857" t="s">
         <v>674</v>
       </c>
@@ -17784,7 +17784,7 @@
       <c r="O10" s="38"/>
     </row>
     <row r="11" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="777" t="s">
+      <c r="A11" s="778" t="s">
         <v>260</v>
       </c>
       <c r="B11" s="711" t="s">
@@ -17813,7 +17813,7 @@
       <c r="O11" s="38"/>
     </row>
     <row r="12" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="777"/>
+      <c r="A12" s="778"/>
       <c r="B12" s="38" t="s">
         <v>9</v>
       </c>
@@ -17840,7 +17840,7 @@
       <c r="O12" s="38"/>
     </row>
     <row r="13" spans="1:15" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="777" t="s">
+      <c r="A13" s="778" t="s">
         <v>68</v>
       </c>
       <c r="B13" s="38" t="s">
@@ -17869,7 +17869,7 @@
       <c r="O13" s="38"/>
     </row>
     <row r="14" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="778" t="s">
+      <c r="A14" s="777" t="s">
         <v>261</v>
       </c>
       <c r="B14" s="102" t="s">
@@ -17898,7 +17898,7 @@
       <c r="O14" s="38"/>
     </row>
     <row r="15" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="777"/>
+      <c r="A15" s="778"/>
       <c r="B15" s="38" t="s">
         <v>281</v>
       </c>
@@ -17925,7 +17925,7 @@
       <c r="O15" s="38"/>
     </row>
     <row r="16" spans="1:15" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="777" t="s">
+      <c r="A16" s="778" t="s">
         <v>68</v>
       </c>
       <c r="B16" s="38" t="s">
@@ -17954,7 +17954,7 @@
       <c r="O16" s="38"/>
     </row>
     <row r="17" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="778" t="s">
+      <c r="A17" s="777" t="s">
         <v>267</v>
       </c>
       <c r="B17" s="102" t="s">
@@ -17983,7 +17983,7 @@
       <c r="O17" s="38"/>
     </row>
     <row r="18" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="777"/>
+      <c r="A18" s="778"/>
       <c r="B18" s="38" t="s">
         <v>281</v>
       </c>
@@ -18010,7 +18010,7 @@
       <c r="O18" s="38"/>
     </row>
     <row r="19" spans="1:15" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="779" t="s">
+      <c r="A19" s="783" t="s">
         <v>68</v>
       </c>
       <c r="B19" s="103" t="s">
@@ -18039,7 +18039,7 @@
       <c r="O19" s="38"/>
     </row>
     <row r="20" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="826" t="s">
+      <c r="A20" s="825" t="s">
         <v>268</v>
       </c>
       <c r="B20" s="75" t="s">
@@ -18068,7 +18068,7 @@
       <c r="O20" s="38"/>
     </row>
     <row r="21" spans="1:15" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="826"/>
+      <c r="A21" s="825"/>
       <c r="B21" s="75" t="s">
         <v>291</v>
       </c>
@@ -18095,7 +18095,7 @@
       <c r="O21" s="38"/>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A22" s="772" t="s">
+      <c r="A22" s="784" t="s">
         <v>94</v>
       </c>
       <c r="B22" s="102" t="s">
@@ -18124,7 +18124,7 @@
       <c r="O22" s="38"/>
     </row>
     <row r="23" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="773"/>
+      <c r="A23" s="789"/>
       <c r="B23" s="38" t="s">
         <v>96</v>
       </c>
@@ -18151,7 +18151,7 @@
       <c r="O23" s="38"/>
     </row>
     <row r="24" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="773"/>
+      <c r="A24" s="789"/>
       <c r="B24" s="38" t="s">
         <v>133</v>
       </c>
@@ -18178,7 +18178,7 @@
       <c r="O24" s="38"/>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A25" s="773"/>
+      <c r="A25" s="789"/>
       <c r="B25" s="38" t="s">
         <v>97</v>
       </c>
@@ -18205,7 +18205,7 @@
       <c r="O25" s="38"/>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A26" s="773"/>
+      <c r="A26" s="789"/>
       <c r="B26" s="38" t="s">
         <v>134</v>
       </c>
@@ -18232,7 +18232,7 @@
       <c r="O26" s="38"/>
     </row>
     <row r="27" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="780"/>
+      <c r="A27" s="785"/>
       <c r="B27" s="103" t="s">
         <v>99</v>
       </c>
@@ -18316,25 +18316,25 @@
       <c r="N1" s="38"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2" s="864" t="s">
+      <c r="A2" s="861" t="s">
         <v>44</v>
       </c>
-      <c r="B2" s="864"/>
-      <c r="C2" s="864"/>
-      <c r="D2" s="864"/>
-      <c r="E2" s="864"/>
-      <c r="F2" s="864"/>
-      <c r="G2" s="864"/>
-      <c r="H2" s="864"/>
-      <c r="I2" s="864"/>
-      <c r="J2" s="864"/>
+      <c r="B2" s="861"/>
+      <c r="C2" s="861"/>
+      <c r="D2" s="861"/>
+      <c r="E2" s="861"/>
+      <c r="F2" s="861"/>
+      <c r="G2" s="861"/>
+      <c r="H2" s="861"/>
+      <c r="I2" s="861"/>
+      <c r="J2" s="861"/>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A3" s="865" t="s">
+      <c r="A3" s="862" t="s">
         <v>349</v>
       </c>
-      <c r="B3" s="866"/>
-      <c r="C3" s="866"/>
+      <c r="B3" s="863"/>
+      <c r="C3" s="863"/>
       <c r="D3" s="185"/>
       <c r="E3" s="185"/>
       <c r="F3" s="185"/>
@@ -18419,18 +18419,18 @@
       <c r="B7" s="182"/>
       <c r="C7" s="182"/>
       <c r="D7" s="182"/>
-      <c r="E7" s="861" t="s">
+      <c r="E7" s="866" t="s">
         <v>64</v>
       </c>
-      <c r="F7" s="862"/>
-      <c r="G7" s="861" t="s">
+      <c r="F7" s="865"/>
+      <c r="G7" s="866" t="s">
         <v>65</v>
       </c>
-      <c r="H7" s="862"/>
-      <c r="I7" s="863" t="s">
+      <c r="H7" s="865"/>
+      <c r="I7" s="864" t="s">
         <v>66</v>
       </c>
-      <c r="J7" s="862"/>
+      <c r="J7" s="865"/>
     </row>
     <row r="8" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="184" t="s">
@@ -19046,18 +19046,18 @@
       <c r="B26" s="182"/>
       <c r="C26" s="182"/>
       <c r="D26" s="182"/>
-      <c r="E26" s="861" t="s">
+      <c r="E26" s="866" t="s">
         <v>64</v>
       </c>
-      <c r="F26" s="862"/>
-      <c r="G26" s="861" t="s">
+      <c r="F26" s="865"/>
+      <c r="G26" s="866" t="s">
         <v>65</v>
       </c>
-      <c r="H26" s="862"/>
-      <c r="I26" s="863" t="s">
+      <c r="H26" s="865"/>
+      <c r="I26" s="864" t="s">
         <v>66</v>
       </c>
-      <c r="J26" s="862"/>
+      <c r="J26" s="865"/>
     </row>
     <row r="27" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="184" t="s">
@@ -19659,18 +19659,18 @@
       <c r="B45" s="182"/>
       <c r="C45" s="182"/>
       <c r="D45" s="182"/>
-      <c r="E45" s="861" t="s">
+      <c r="E45" s="866" t="s">
         <v>64</v>
       </c>
-      <c r="F45" s="862"/>
-      <c r="G45" s="861" t="s">
+      <c r="F45" s="865"/>
+      <c r="G45" s="866" t="s">
         <v>65</v>
       </c>
-      <c r="H45" s="862"/>
-      <c r="I45" s="863" t="s">
+      <c r="H45" s="865"/>
+      <c r="I45" s="864" t="s">
         <v>66</v>
       </c>
-      <c r="J45" s="862"/>
+      <c r="J45" s="865"/>
     </row>
     <row r="46" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="184" t="s">
@@ -20265,18 +20265,18 @@
       <c r="B64" s="182"/>
       <c r="C64" s="182"/>
       <c r="D64" s="182"/>
-      <c r="E64" s="861" t="s">
+      <c r="E64" s="866" t="s">
         <v>64</v>
       </c>
-      <c r="F64" s="862"/>
-      <c r="G64" s="861" t="s">
+      <c r="F64" s="865"/>
+      <c r="G64" s="866" t="s">
         <v>65</v>
       </c>
-      <c r="H64" s="862"/>
-      <c r="I64" s="863" t="s">
+      <c r="H64" s="865"/>
+      <c r="I64" s="864" t="s">
         <v>66</v>
       </c>
-      <c r="J64" s="862"/>
+      <c r="J64" s="865"/>
     </row>
     <row r="65" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A65" s="184" t="s">
@@ -20664,18 +20664,18 @@
       <c r="B77" s="182"/>
       <c r="C77" s="182"/>
       <c r="D77" s="182"/>
-      <c r="E77" s="861" t="s">
+      <c r="E77" s="866" t="s">
         <v>64</v>
       </c>
-      <c r="F77" s="862"/>
-      <c r="G77" s="861" t="s">
+      <c r="F77" s="865"/>
+      <c r="G77" s="866" t="s">
         <v>65</v>
       </c>
-      <c r="H77" s="862"/>
-      <c r="I77" s="863" t="s">
+      <c r="H77" s="865"/>
+      <c r="I77" s="864" t="s">
         <v>66</v>
       </c>
-      <c r="J77" s="862"/>
+      <c r="J77" s="865"/>
     </row>
     <row r="78" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A78" s="184" t="s">
@@ -21058,11 +21058,6 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A3:C3"/>
-    <mergeCell ref="I45:J45"/>
-    <mergeCell ref="G26:H26"/>
-    <mergeCell ref="I26:J26"/>
     <mergeCell ref="G77:H77"/>
     <mergeCell ref="I77:J77"/>
     <mergeCell ref="E7:F7"/>
@@ -21075,6 +21070,11 @@
     <mergeCell ref="G45:H45"/>
     <mergeCell ref="G7:H7"/>
     <mergeCell ref="I7:J7"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="I45:J45"/>
+    <mergeCell ref="G26:H26"/>
+    <mergeCell ref="I26:J26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -21086,7 +21086,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:N65"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A17" workbookViewId="0">
       <selection activeCell="E37" sqref="E37"/>
     </sheetView>
   </sheetViews>
@@ -22320,18 +22320,21 @@
   </sheetPr>
   <dimension ref="A1:S93"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="7" topLeftCell="E65" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
+      <pane xSplit="3" ySplit="7" topLeftCell="F66" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
-      <selection pane="bottomRight" activeCell="E86" sqref="E86"/>
+      <selection pane="bottomRight" activeCell="F73" sqref="F73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="38.140625" style="38" customWidth="1"/>
+    <col min="1" max="1" width="54.140625" style="38" customWidth="1"/>
     <col min="2" max="2" width="22.42578125" style="38" bestFit="1" customWidth="1"/>
-    <col min="3" max="6" width="40.140625" style="38" customWidth="1"/>
+    <col min="3" max="3" width="33.42578125" style="38" customWidth="1"/>
+    <col min="4" max="4" width="28.28515625" style="38" customWidth="1"/>
+    <col min="5" max="5" width="30.85546875" style="38" customWidth="1"/>
+    <col min="6" max="6" width="40.140625" style="38" customWidth="1"/>
     <col min="7" max="9" width="21.7109375" style="38" customWidth="1"/>
     <col min="10" max="10" width="108.140625" style="38" bestFit="1" customWidth="1"/>
     <col min="11" max="19" width="8.85546875" style="38"/>
@@ -22374,18 +22377,18 @@
       <c r="A5" s="120"/>
       <c r="B5" s="121"/>
       <c r="C5" s="121"/>
-      <c r="D5" s="785" t="s">
+      <c r="D5" s="775" t="s">
         <v>474</v>
       </c>
-      <c r="E5" s="786"/>
-      <c r="F5" s="785" t="s">
+      <c r="E5" s="776"/>
+      <c r="F5" s="775" t="s">
         <v>472</v>
       </c>
-      <c r="G5" s="786"/>
-      <c r="H5" s="785" t="s">
+      <c r="G5" s="776"/>
+      <c r="H5" s="775" t="s">
         <v>473</v>
       </c>
-      <c r="I5" s="786"/>
+      <c r="I5" s="776"/>
       <c r="J5" s="770" t="s">
         <v>15</v>
       </c>
@@ -22405,18 +22408,18 @@
       </c>
       <c r="B6" s="127"/>
       <c r="C6" s="128"/>
-      <c r="D6" s="787" t="s">
+      <c r="D6" s="779" t="s">
         <v>475</v>
       </c>
-      <c r="E6" s="788"/>
-      <c r="F6" s="789" t="s">
+      <c r="E6" s="780"/>
+      <c r="F6" s="781" t="s">
         <v>468</v>
       </c>
-      <c r="G6" s="790"/>
-      <c r="H6" s="789" t="s">
+      <c r="G6" s="782"/>
+      <c r="H6" s="781" t="s">
         <v>469</v>
       </c>
-      <c r="I6" s="790"/>
+      <c r="I6" s="782"/>
       <c r="J6" s="62"/>
       <c r="K6" s="63"/>
       <c r="L6" s="63"/>
@@ -22511,7 +22514,7 @@
       <c r="S8" s="118"/>
     </row>
     <row r="9" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="778" t="s">
+      <c r="A9" s="777" t="s">
         <v>1</v>
       </c>
       <c r="B9" s="102" t="s">
@@ -22547,7 +22550,7 @@
       </c>
     </row>
     <row r="10" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="777"/>
+      <c r="A10" s="778"/>
       <c r="B10" s="38" t="s">
         <v>12</v>
       </c>
@@ -22581,7 +22584,7 @@
       </c>
     </row>
     <row r="11" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="777"/>
+      <c r="A11" s="778"/>
       <c r="B11" s="38" t="s">
         <v>13</v>
       </c>
@@ -22614,7 +22617,7 @@
       </c>
     </row>
     <row r="12" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="777"/>
+      <c r="A12" s="778"/>
       <c r="B12" s="38" t="s">
         <v>37</v>
       </c>
@@ -22648,7 +22651,7 @@
       </c>
     </row>
     <row r="13" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="778" t="s">
+      <c r="A13" s="777" t="s">
         <v>41</v>
       </c>
       <c r="B13" s="102" t="s">
@@ -22684,7 +22687,7 @@
       </c>
     </row>
     <row r="14" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="779"/>
+      <c r="A14" s="783"/>
       <c r="B14" s="103" t="s">
         <v>9</v>
       </c>
@@ -22718,7 +22721,7 @@
       </c>
     </row>
     <row r="15" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="778" t="s">
+      <c r="A15" s="777" t="s">
         <v>21</v>
       </c>
       <c r="B15" s="102" t="s">
@@ -22754,7 +22757,7 @@
       </c>
     </row>
     <row r="16" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="779"/>
+      <c r="A16" s="783"/>
       <c r="B16" s="103" t="s">
         <v>319</v>
       </c>
@@ -22867,7 +22870,7 @@
       <c r="S18" s="118"/>
     </row>
     <row r="19" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="778" t="s">
+      <c r="A19" s="777" t="s">
         <v>22</v>
       </c>
       <c r="B19" s="102" t="s">
@@ -22903,7 +22906,7 @@
       </c>
     </row>
     <row r="20" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="779"/>
+      <c r="A20" s="783"/>
       <c r="B20" s="103" t="s">
         <v>319</v>
       </c>
@@ -22937,7 +22940,7 @@
       </c>
     </row>
     <row r="21" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="777" t="s">
+      <c r="A21" s="778" t="s">
         <v>23</v>
       </c>
       <c r="B21" s="102" t="s">
@@ -22973,7 +22976,7 @@
       </c>
     </row>
     <row r="22" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="779"/>
+      <c r="A22" s="783"/>
       <c r="B22" s="103" t="s">
         <v>319</v>
       </c>
@@ -23084,7 +23087,7 @@
       <c r="S24" s="118"/>
     </row>
     <row r="25" spans="1:19" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="778" t="s">
+      <c r="A25" s="777" t="s">
         <v>149</v>
       </c>
       <c r="B25" s="102" t="s">
@@ -23131,7 +23134,7 @@
       <c r="S25" s="26"/>
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A26" s="777"/>
+      <c r="A26" s="778"/>
       <c r="B26" s="38" t="s">
         <v>9</v>
       </c>
@@ -23176,7 +23179,7 @@
       <c r="S26" s="26"/>
     </row>
     <row r="27" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="779"/>
+      <c r="A27" s="783"/>
       <c r="B27" s="103" t="s">
         <v>7</v>
       </c>
@@ -23268,7 +23271,7 @@
       <c r="S28" s="26"/>
     </row>
     <row r="29" spans="1:19" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="778" t="s">
+      <c r="A29" s="777" t="s">
         <v>38</v>
       </c>
       <c r="B29" s="102" t="s">
@@ -23315,7 +23318,7 @@
       <c r="S29" s="26"/>
     </row>
     <row r="30" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A30" s="777"/>
+      <c r="A30" s="778"/>
       <c r="B30" s="38" t="s">
         <v>9</v>
       </c>
@@ -23360,7 +23363,7 @@
       <c r="S30" s="26"/>
     </row>
     <row r="31" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="779"/>
+      <c r="A31" s="783"/>
       <c r="B31" s="103" t="s">
         <v>7</v>
       </c>
@@ -23405,7 +23408,7 @@
       <c r="S31" s="26"/>
     </row>
     <row r="32" spans="1:19" s="38" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="772" t="s">
+      <c r="A32" s="784" t="s">
         <v>0</v>
       </c>
       <c r="B32" s="102" t="s">
@@ -23443,7 +23446,7 @@
       </c>
     </row>
     <row r="33" spans="1:19" s="38" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="773"/>
+      <c r="A33" s="789"/>
       <c r="B33" s="38" t="s">
         <v>9</v>
       </c>
@@ -23479,7 +23482,7 @@
       </c>
     </row>
     <row r="34" spans="1:19" s="38" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="773"/>
+      <c r="A34" s="789"/>
       <c r="B34" s="38" t="s">
         <v>7</v>
       </c>
@@ -23515,7 +23518,7 @@
       </c>
     </row>
     <row r="35" spans="1:19" s="38" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="780"/>
+      <c r="A35" s="785"/>
       <c r="B35" s="103" t="s">
         <v>20</v>
       </c>
@@ -23681,7 +23684,7 @@
       <c r="S38" s="26"/>
     </row>
     <row r="39" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A39" s="775" t="s">
+      <c r="A39" s="786" t="s">
         <v>27</v>
       </c>
       <c r="B39" s="102" t="s">
@@ -23727,7 +23730,7 @@
       <c r="S39" s="26"/>
     </row>
     <row r="40" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="776"/>
+      <c r="A40" s="790"/>
       <c r="B40" s="103" t="s">
         <v>29</v>
       </c>
@@ -23813,7 +23816,7 @@
       <c r="S41" s="118"/>
     </row>
     <row r="42" spans="1:19" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="772" t="s">
+      <c r="A42" s="784" t="s">
         <v>149</v>
       </c>
       <c r="B42" s="102" t="s">
@@ -23860,7 +23863,7 @@
       <c r="S42" s="26"/>
     </row>
     <row r="43" spans="1:19" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="773"/>
+      <c r="A43" s="789"/>
       <c r="B43" s="38" t="s">
         <v>116</v>
       </c>
@@ -23905,7 +23908,7 @@
       <c r="S43" s="26"/>
     </row>
     <row r="44" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="774"/>
+      <c r="A44" s="787"/>
       <c r="B44" s="38" t="s">
         <v>117</v>
       </c>
@@ -23950,7 +23953,7 @@
       <c r="S44" s="26"/>
     </row>
     <row r="45" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="774"/>
+      <c r="A45" s="787"/>
       <c r="B45" s="38" t="s">
         <v>118</v>
       </c>
@@ -23995,7 +23998,7 @@
       <c r="S45" s="26"/>
     </row>
     <row r="46" spans="1:19" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="772" t="s">
+      <c r="A46" s="784" t="s">
         <v>375</v>
       </c>
       <c r="B46" s="102" t="s">
@@ -24042,7 +24045,7 @@
       <c r="S46" s="26"/>
     </row>
     <row r="47" spans="1:19" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="773"/>
+      <c r="A47" s="789"/>
       <c r="B47" s="38" t="s">
         <v>116</v>
       </c>
@@ -24087,7 +24090,7 @@
       <c r="S47" s="26"/>
     </row>
     <row r="48" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A48" s="774"/>
+      <c r="A48" s="787"/>
       <c r="B48" s="38" t="s">
         <v>117</v>
       </c>
@@ -24132,7 +24135,7 @@
       <c r="S48" s="26"/>
     </row>
     <row r="49" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="774"/>
+      <c r="A49" s="787"/>
       <c r="B49" s="38" t="s">
         <v>118</v>
       </c>
@@ -24177,7 +24180,7 @@
       <c r="S49" s="26"/>
     </row>
     <row r="50" spans="1:19" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="772" t="s">
+      <c r="A50" s="784" t="s">
         <v>374</v>
       </c>
       <c r="B50" s="102" t="s">
@@ -24224,7 +24227,7 @@
       <c r="S50" s="26"/>
     </row>
     <row r="51" spans="1:19" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="773"/>
+      <c r="A51" s="789"/>
       <c r="B51" s="38" t="s">
         <v>116</v>
       </c>
@@ -24269,7 +24272,7 @@
       <c r="S51" s="26"/>
     </row>
     <row r="52" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A52" s="774"/>
+      <c r="A52" s="787"/>
       <c r="B52" s="38" t="s">
         <v>117</v>
       </c>
@@ -24314,7 +24317,7 @@
       <c r="S52" s="26"/>
     </row>
     <row r="53" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="774"/>
+      <c r="A53" s="787"/>
       <c r="B53" s="38" t="s">
         <v>118</v>
       </c>
@@ -24359,7 +24362,7 @@
       <c r="S53" s="26"/>
     </row>
     <row r="54" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A54" s="782" t="s">
+      <c r="A54" s="772" t="s">
         <v>627</v>
       </c>
       <c r="B54" s="630" t="s">
@@ -24403,7 +24406,7 @@
       <c r="S54" s="26"/>
     </row>
     <row r="55" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A55" s="783"/>
+      <c r="A55" s="773"/>
       <c r="B55" s="26" t="s">
         <v>116</v>
       </c>
@@ -24445,7 +24448,7 @@
       <c r="S55" s="26"/>
     </row>
     <row r="56" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A56" s="783"/>
+      <c r="A56" s="773"/>
       <c r="B56" s="26" t="s">
         <v>117</v>
       </c>
@@ -24487,7 +24490,7 @@
       <c r="S56" s="26"/>
     </row>
     <row r="57" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A57" s="784"/>
+      <c r="A57" s="774"/>
       <c r="B57" s="620" t="s">
         <v>118</v>
       </c>
@@ -24529,7 +24532,7 @@
       <c r="S57" s="26"/>
     </row>
     <row r="58" spans="1:19" s="38" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A58" s="777" t="s">
+      <c r="A58" s="778" t="s">
         <v>0</v>
       </c>
       <c r="B58" s="38" t="s">
@@ -24567,7 +24570,7 @@
       </c>
     </row>
     <row r="59" spans="1:19" s="38" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="777"/>
+      <c r="A59" s="778"/>
       <c r="B59" s="38" t="s">
         <v>7</v>
       </c>
@@ -24603,7 +24606,7 @@
       </c>
     </row>
     <row r="60" spans="1:19" s="38" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A60" s="775" t="s">
+      <c r="A60" s="786" t="s">
         <v>17</v>
       </c>
       <c r="B60" s="323" t="s">
@@ -24641,7 +24644,7 @@
       </c>
     </row>
     <row r="61" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A61" s="774"/>
+      <c r="A61" s="787"/>
       <c r="B61" s="38" t="s">
         <v>115</v>
       </c>
@@ -24686,7 +24689,7 @@
       <c r="S61" s="26"/>
     </row>
     <row r="62" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A62" s="774"/>
+      <c r="A62" s="787"/>
       <c r="B62" s="38" t="s">
         <v>116</v>
       </c>
@@ -24731,7 +24734,7 @@
       <c r="S62" s="26"/>
     </row>
     <row r="63" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A63" s="774"/>
+      <c r="A63" s="787"/>
       <c r="B63" s="38" t="s">
         <v>117</v>
       </c>
@@ -24776,7 +24779,7 @@
       <c r="S63" s="26"/>
     </row>
     <row r="64" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A64" s="781"/>
+      <c r="A64" s="788"/>
       <c r="B64" s="103" t="s">
         <v>118</v>
       </c>
@@ -24899,7 +24902,7 @@
       <c r="K66" s="771"/>
     </row>
     <row r="67" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A67" s="772" t="s">
+      <c r="A67" s="784" t="s">
         <v>307</v>
       </c>
       <c r="B67" s="102" t="s">
@@ -24937,7 +24940,7 @@
       </c>
     </row>
     <row r="68" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A68" s="780"/>
+      <c r="A68" s="785"/>
       <c r="B68" s="103" t="s">
         <v>7</v>
       </c>
@@ -25470,6 +25473,20 @@
     <protectedRange algorithmName="SHA-512" hashValue="bhbLMjBtLJkCl6+oRAIq98NZkcBAWzm8GjbRfoftLGnxxPl6tbwDiFe+9aTX2EHNMDT88cd1rnVmqQcow+/x8w==" saltValue="u4cWX+yqQiFBZXUHKrq6Og==" spinCount="100000" sqref="F9:G23" name="Indata"/>
   </protectedRanges>
   <mergeCells count="30">
+    <mergeCell ref="J66:K66"/>
+    <mergeCell ref="A42:A45"/>
+    <mergeCell ref="A46:A49"/>
+    <mergeCell ref="A50:A53"/>
+    <mergeCell ref="A39:A40"/>
+    <mergeCell ref="A58:A59"/>
+    <mergeCell ref="A19:A20"/>
+    <mergeCell ref="A21:A22"/>
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="A25:A27"/>
+    <mergeCell ref="A67:A68"/>
+    <mergeCell ref="A60:A64"/>
+    <mergeCell ref="A29:A31"/>
+    <mergeCell ref="A32:A35"/>
     <mergeCell ref="J69:K69"/>
     <mergeCell ref="A54:A57"/>
     <mergeCell ref="D5:E5"/>
@@ -25486,20 +25503,6 @@
     <mergeCell ref="J18:K18"/>
     <mergeCell ref="J24:K24"/>
     <mergeCell ref="A13:A14"/>
-    <mergeCell ref="A19:A20"/>
-    <mergeCell ref="A21:A22"/>
-    <mergeCell ref="A15:A16"/>
-    <mergeCell ref="A25:A27"/>
-    <mergeCell ref="A67:A68"/>
-    <mergeCell ref="A60:A64"/>
-    <mergeCell ref="A29:A31"/>
-    <mergeCell ref="A32:A35"/>
-    <mergeCell ref="J66:K66"/>
-    <mergeCell ref="A42:A45"/>
-    <mergeCell ref="A46:A49"/>
-    <mergeCell ref="A50:A53"/>
-    <mergeCell ref="A39:A40"/>
-    <mergeCell ref="A58:A59"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -25533,7 +25536,7 @@
   <dimension ref="B2:E35"/>
   <sheetViews>
     <sheetView topLeftCell="A16" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -25853,7 +25856,7 @@
   <dimension ref="B1:I8"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -26014,8 +26017,8 @@
   </sheetPr>
   <dimension ref="A1:AM89"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+    <sheetView topLeftCell="K1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <pane ySplit="4" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="Q16" sqref="Q16"/>
     </sheetView>
   </sheetViews>
@@ -26053,10 +26056,10 @@
       <c r="A3" s="791" t="s">
         <v>67</v>
       </c>
-      <c r="B3" s="808" t="s">
+      <c r="B3" s="798" t="s">
         <v>222</v>
       </c>
-      <c r="C3" s="809"/>
+      <c r="C3" s="799"/>
       <c r="D3" s="791" t="s">
         <v>64</v>
       </c>
@@ -26072,10 +26075,10 @@
       <c r="K3" s="791" t="s">
         <v>67</v>
       </c>
-      <c r="L3" s="803" t="s">
+      <c r="L3" s="802" t="s">
         <v>232</v>
       </c>
-      <c r="M3" s="804"/>
+      <c r="M3" s="803"/>
       <c r="N3" s="791" t="s">
         <v>64</v>
       </c>
@@ -26091,10 +26094,10 @@
       <c r="U3" s="791" t="s">
         <v>67</v>
       </c>
-      <c r="V3" s="803" t="s">
+      <c r="V3" s="802" t="s">
         <v>223</v>
       </c>
-      <c r="W3" s="804"/>
+      <c r="W3" s="803"/>
       <c r="X3" s="791" t="s">
         <v>64</v>
       </c>
@@ -26110,10 +26113,10 @@
       <c r="AE3" s="791" t="s">
         <v>67</v>
       </c>
-      <c r="AF3" s="803" t="s">
+      <c r="AF3" s="802" t="s">
         <v>233</v>
       </c>
-      <c r="AG3" s="804"/>
+      <c r="AG3" s="803"/>
       <c r="AH3" s="791" t="s">
         <v>64</v>
       </c>
@@ -26128,9 +26131,9 @@
       <c r="AM3" s="792"/>
     </row>
     <row r="4" spans="1:39" s="118" customFormat="1" ht="25.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="807"/>
-      <c r="B4" s="810"/>
-      <c r="C4" s="811"/>
+      <c r="A4" s="797"/>
+      <c r="B4" s="800"/>
+      <c r="C4" s="801"/>
       <c r="D4" s="253">
         <v>2030</v>
       </c>
@@ -26149,9 +26152,9 @@
       <c r="I4" s="254">
         <v>2040</v>
       </c>
-      <c r="K4" s="807"/>
-      <c r="L4" s="805"/>
-      <c r="M4" s="806"/>
+      <c r="K4" s="797"/>
+      <c r="L4" s="804"/>
+      <c r="M4" s="805"/>
       <c r="N4" s="253">
         <v>2030</v>
       </c>
@@ -26170,9 +26173,9 @@
       <c r="S4" s="254">
         <v>2040</v>
       </c>
-      <c r="U4" s="807"/>
-      <c r="V4" s="805"/>
-      <c r="W4" s="806"/>
+      <c r="U4" s="797"/>
+      <c r="V4" s="804"/>
+      <c r="W4" s="805"/>
       <c r="X4" s="253">
         <v>2030</v>
       </c>
@@ -26191,9 +26194,9 @@
       <c r="AC4" s="254">
         <v>2040</v>
       </c>
-      <c r="AE4" s="807"/>
-      <c r="AF4" s="805"/>
-      <c r="AG4" s="806"/>
+      <c r="AE4" s="797"/>
+      <c r="AF4" s="804"/>
+      <c r="AG4" s="805"/>
       <c r="AH4" s="253">
         <v>2030</v>
       </c>
@@ -26254,7 +26257,7 @@
       <c r="AM5" s="189"/>
     </row>
     <row r="6" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A6" s="797" t="s">
+      <c r="A6" s="806" t="s">
         <v>0</v>
       </c>
       <c r="B6" s="124" t="s">
@@ -26287,7 +26290,7 @@
         <f>Indata!I32</f>
         <v>21.293751803814949</v>
       </c>
-      <c r="K6" s="797" t="s">
+      <c r="K6" s="806" t="s">
         <v>0</v>
       </c>
       <c r="L6" s="124" t="s">
@@ -26320,7 +26323,7 @@
         <f>'Modell - Drivmedelpriser'!J24</f>
         <v>21.293751803814949</v>
       </c>
-      <c r="U6" s="797" t="s">
+      <c r="U6" s="806" t="s">
         <v>0</v>
       </c>
       <c r="V6" s="124" t="s">
@@ -26353,7 +26356,7 @@
         <f t="shared" ref="AC6:AC8" si="4">S6</f>
         <v>21.293751803814949</v>
       </c>
-      <c r="AE6" s="797" t="s">
+      <c r="AE6" s="806" t="s">
         <v>0</v>
       </c>
       <c r="AF6" s="124" t="s">
@@ -26388,7 +26391,7 @@
       </c>
     </row>
     <row r="7" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A7" s="798"/>
+      <c r="A7" s="807"/>
       <c r="B7" s="125" t="s">
         <v>9</v>
       </c>
@@ -26419,7 +26422,7 @@
         <f>Indata!I33</f>
         <v>22.557131724953557</v>
       </c>
-      <c r="K7" s="798"/>
+      <c r="K7" s="807"/>
       <c r="L7" s="125" t="s">
         <v>9</v>
       </c>
@@ -26450,7 +26453,7 @@
         <f>'Modell - Drivmedelpriser'!J43</f>
         <v>22.557131724953557</v>
       </c>
-      <c r="U7" s="798"/>
+      <c r="U7" s="807"/>
       <c r="V7" s="125" t="s">
         <v>9</v>
       </c>
@@ -26481,7 +26484,7 @@
         <f t="shared" si="4"/>
         <v>22.557131724953557</v>
       </c>
-      <c r="AE7" s="798"/>
+      <c r="AE7" s="807"/>
       <c r="AF7" s="125" t="s">
         <v>9</v>
       </c>
@@ -26514,7 +26517,7 @@
       </c>
     </row>
     <row r="8" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A8" s="798"/>
+      <c r="A8" s="807"/>
       <c r="B8" s="125" t="s">
         <v>7</v>
       </c>
@@ -26545,7 +26548,7 @@
         <f>Indata!I34</f>
         <v>4.1598749999999995</v>
       </c>
-      <c r="K8" s="798"/>
+      <c r="K8" s="807"/>
       <c r="L8" s="125" t="s">
         <v>7</v>
       </c>
@@ -26576,7 +26579,7 @@
         <f>'Modell - Drivmedelpriser'!J75</f>
         <v>4.1598749999999995</v>
       </c>
-      <c r="U8" s="798"/>
+      <c r="U8" s="807"/>
       <c r="V8" s="125" t="s">
         <v>7</v>
       </c>
@@ -26607,7 +26610,7 @@
         <f t="shared" si="4"/>
         <v>4.1598749999999995</v>
       </c>
-      <c r="AE8" s="798"/>
+      <c r="AE8" s="807"/>
       <c r="AF8" s="125" t="s">
         <v>7</v>
       </c>
@@ -26640,7 +26643,7 @@
       </c>
     </row>
     <row r="9" spans="1:39" s="290" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="798"/>
+      <c r="A9" s="807"/>
       <c r="B9" s="175" t="s">
         <v>20</v>
       </c>
@@ -26671,7 +26674,7 @@
         <f>Indata!I35</f>
         <v>21.927924171466245</v>
       </c>
-      <c r="K9" s="798"/>
+      <c r="K9" s="807"/>
       <c r="L9" s="175" t="s">
         <v>20</v>
       </c>
@@ -26702,7 +26705,7 @@
         <f t="shared" si="12"/>
         <v>21.927924171466245</v>
       </c>
-      <c r="U9" s="798"/>
+      <c r="U9" s="807"/>
       <c r="V9" s="175" t="s">
         <v>20</v>
       </c>
@@ -26733,7 +26736,7 @@
         <f t="shared" si="13"/>
         <v>21.927924171466245</v>
       </c>
-      <c r="AE9" s="798"/>
+      <c r="AE9" s="807"/>
       <c r="AF9" s="175" t="s">
         <v>20</v>
       </c>
@@ -26766,7 +26769,7 @@
       </c>
     </row>
     <row r="10" spans="1:39" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="799"/>
+      <c r="A10" s="808"/>
       <c r="B10" s="176" t="s">
         <v>229</v>
       </c>
@@ -26791,7 +26794,7 @@
       <c r="I10" s="213" t="s">
         <v>78</v>
       </c>
-      <c r="K10" s="799"/>
+      <c r="K10" s="808"/>
       <c r="L10" s="176" t="s">
         <v>229</v>
       </c>
@@ -26822,7 +26825,7 @@
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
-      <c r="U10" s="799"/>
+      <c r="U10" s="808"/>
       <c r="V10" s="176" t="s">
         <v>229</v>
       </c>
@@ -26853,7 +26856,7 @@
         <f t="shared" si="16"/>
         <v>0</v>
       </c>
-      <c r="AE10" s="799"/>
+      <c r="AE10" s="808"/>
       <c r="AF10" s="176" t="s">
         <v>229</v>
       </c>
@@ -26955,7 +26958,7 @@
       <c r="AM12" s="189"/>
     </row>
     <row r="13" spans="1:39" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="797" t="s">
+      <c r="A13" s="806" t="s">
         <v>38</v>
       </c>
       <c r="B13" s="124" t="s">
@@ -26988,7 +26991,7 @@
         <f>Indata!I29</f>
         <v>0.49219920755019081</v>
       </c>
-      <c r="K13" s="800" t="s">
+      <c r="K13" s="809" t="s">
         <v>38</v>
       </c>
       <c r="L13" s="659" t="s">
@@ -27021,7 +27024,7 @@
         <f>I13*(100%+S$10*'Indata - Effektsamband-Faktorer'!$E$5)*(1-Indata!I$19)*(1-I52*Indata!I75)</f>
         <v>0.49219920755019081</v>
       </c>
-      <c r="U13" s="797" t="s">
+      <c r="U13" s="806" t="s">
         <v>38</v>
       </c>
       <c r="V13" s="124" t="s">
@@ -27054,7 +27057,7 @@
         <f t="shared" ref="AC13:AC15" si="22">S13</f>
         <v>0.49219920755019081</v>
       </c>
-      <c r="AE13" s="797" t="s">
+      <c r="AE13" s="806" t="s">
         <v>38</v>
       </c>
       <c r="AF13" s="124" t="s">
@@ -27089,7 +27092,7 @@
       </c>
     </row>
     <row r="14" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A14" s="798"/>
+      <c r="A14" s="807"/>
       <c r="B14" s="125" t="s">
         <v>9</v>
       </c>
@@ -27120,7 +27123,7 @@
         <f>Indata!I30</f>
         <v>0.49160078067679608</v>
       </c>
-      <c r="K14" s="801"/>
+      <c r="K14" s="810"/>
       <c r="L14" s="660" t="s">
         <v>9</v>
       </c>
@@ -27151,7 +27154,7 @@
         <f>I14*(100%+S$10*'Indata - Effektsamband-Faktorer'!$E$5)*(1-Indata!I$19)*(1-I52*Indata!I75)</f>
         <v>0.49160078067679608</v>
       </c>
-      <c r="U14" s="798"/>
+      <c r="U14" s="807"/>
       <c r="V14" s="125" t="s">
         <v>9</v>
       </c>
@@ -27182,7 +27185,7 @@
         <f t="shared" si="22"/>
         <v>0.49160078067679608</v>
       </c>
-      <c r="AE14" s="798"/>
+      <c r="AE14" s="807"/>
       <c r="AF14" s="125" t="s">
         <v>9</v>
       </c>
@@ -27215,7 +27218,7 @@
       </c>
     </row>
     <row r="15" spans="1:39" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="799"/>
+      <c r="A15" s="808"/>
       <c r="B15" s="126" t="s">
         <v>7</v>
       </c>
@@ -27246,7 +27249,7 @@
         <f>Indata!I31</f>
         <v>1.6150000000000002</v>
       </c>
-      <c r="K15" s="802"/>
+      <c r="K15" s="811"/>
       <c r="L15" s="661" t="s">
         <v>7</v>
       </c>
@@ -27277,7 +27280,7 @@
         <f>I15*(1-Indata!I$19)*(1-I52*Indata!I75)</f>
         <v>1.6150000000000002</v>
       </c>
-      <c r="U15" s="799"/>
+      <c r="U15" s="808"/>
       <c r="V15" s="126" t="s">
         <v>7</v>
       </c>
@@ -27308,7 +27311,7 @@
         <f t="shared" si="22"/>
         <v>1.6150000000000002</v>
       </c>
-      <c r="AE15" s="799"/>
+      <c r="AE15" s="808"/>
       <c r="AF15" s="126" t="s">
         <v>7</v>
       </c>
@@ -27991,7 +27994,7 @@
       <c r="AM23" s="189"/>
     </row>
     <row r="24" spans="1:39" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="797" t="s">
+      <c r="A24" s="806" t="s">
         <v>21</v>
       </c>
       <c r="B24" s="124" t="s">
@@ -28024,7 +28027,7 @@
         <f>Indata!I$15*10</f>
         <v>0</v>
       </c>
-      <c r="K24" s="797" t="s">
+      <c r="K24" s="806" t="s">
         <v>21</v>
       </c>
       <c r="L24" s="124" t="s">
@@ -28057,7 +28060,7 @@
         <f t="shared" si="45"/>
         <v>0</v>
       </c>
-      <c r="U24" s="797" t="s">
+      <c r="U24" s="806" t="s">
         <v>21</v>
       </c>
       <c r="V24" s="124" t="s">
@@ -28090,7 +28093,7 @@
         <f t="shared" ref="AC24:AC26" si="50">S24</f>
         <v>0</v>
       </c>
-      <c r="AE24" s="797" t="s">
+      <c r="AE24" s="806" t="s">
         <v>21</v>
       </c>
       <c r="AF24" s="124" t="s">
@@ -28125,7 +28128,7 @@
       </c>
     </row>
     <row r="25" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A25" s="798"/>
+      <c r="A25" s="807"/>
       <c r="B25" s="125" t="s">
         <v>9</v>
       </c>
@@ -28156,7 +28159,7 @@
         <f>Indata!I$15*10</f>
         <v>0</v>
       </c>
-      <c r="K25" s="798"/>
+      <c r="K25" s="807"/>
       <c r="L25" s="125" t="s">
         <v>9</v>
       </c>
@@ -28187,7 +28190,7 @@
         <f t="shared" ref="S25:S26" si="61">I25</f>
         <v>0</v>
       </c>
-      <c r="U25" s="798"/>
+      <c r="U25" s="807"/>
       <c r="V25" s="125" t="s">
         <v>9</v>
       </c>
@@ -28218,7 +28221,7 @@
         <f t="shared" si="50"/>
         <v>0</v>
       </c>
-      <c r="AE25" s="798"/>
+      <c r="AE25" s="807"/>
       <c r="AF25" s="125" t="s">
         <v>9</v>
       </c>
@@ -28251,7 +28254,7 @@
       </c>
     </row>
     <row r="26" spans="1:39" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="799"/>
+      <c r="A26" s="808"/>
       <c r="B26" s="126" t="s">
         <v>7</v>
       </c>
@@ -28282,7 +28285,7 @@
         <f>Indata!I$15*10</f>
         <v>0</v>
       </c>
-      <c r="K26" s="799"/>
+      <c r="K26" s="808"/>
       <c r="L26" s="126" t="s">
         <v>7</v>
       </c>
@@ -28313,7 +28316,7 @@
         <f t="shared" si="61"/>
         <v>0</v>
       </c>
-      <c r="U26" s="799"/>
+      <c r="U26" s="808"/>
       <c r="V26" s="126" t="s">
         <v>7</v>
       </c>
@@ -28344,7 +28347,7 @@
         <f t="shared" si="50"/>
         <v>0</v>
       </c>
-      <c r="AE26" s="799"/>
+      <c r="AE26" s="808"/>
       <c r="AF26" s="126" t="s">
         <v>7</v>
       </c>
@@ -28452,7 +28455,7 @@
       <c r="AM28" s="189"/>
     </row>
     <row r="29" spans="1:39" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="797" t="s">
+      <c r="A29" s="806" t="s">
         <v>75</v>
       </c>
       <c r="B29" s="124" t="s">
@@ -28485,7 +28488,7 @@
         <f>Indata!I$36</f>
         <v>10.009999999999998</v>
       </c>
-      <c r="K29" s="800" t="s">
+      <c r="K29" s="809" t="s">
         <v>75</v>
       </c>
       <c r="L29" s="659" t="s">
@@ -28518,7 +28521,7 @@
         <f>I29*(1-Indata!I$74)+I29*(1+Indata!I$76)*I$52</f>
         <v>10.009999999999998</v>
       </c>
-      <c r="U29" s="797" t="s">
+      <c r="U29" s="806" t="s">
         <v>75</v>
       </c>
       <c r="V29" s="124" t="s">
@@ -28551,7 +28554,7 @@
         <f t="shared" ref="AC29:AC31" si="68">S29</f>
         <v>10.009999999999998</v>
       </c>
-      <c r="AE29" s="797" t="s">
+      <c r="AE29" s="806" t="s">
         <v>75</v>
       </c>
       <c r="AF29" s="124" t="s">
@@ -28586,7 +28589,7 @@
       </c>
     </row>
     <row r="30" spans="1:39" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="798"/>
+      <c r="A30" s="807"/>
       <c r="B30" s="125" t="s">
         <v>9</v>
       </c>
@@ -28617,7 +28620,7 @@
         <f>Indata!I$36</f>
         <v>10.009999999999998</v>
       </c>
-      <c r="K30" s="801"/>
+      <c r="K30" s="810"/>
       <c r="L30" s="660" t="s">
         <v>9</v>
       </c>
@@ -28648,7 +28651,7 @@
         <f>I30*(1-Indata!I$74)+I30*(1+Indata!I$76)*I$52</f>
         <v>10.009999999999998</v>
       </c>
-      <c r="U30" s="798"/>
+      <c r="U30" s="807"/>
       <c r="V30" s="125" t="s">
         <v>9</v>
       </c>
@@ -28679,7 +28682,7 @@
         <f t="shared" si="68"/>
         <v>10.009999999999998</v>
       </c>
-      <c r="AE30" s="798"/>
+      <c r="AE30" s="807"/>
       <c r="AF30" s="125" t="s">
         <v>9</v>
       </c>
@@ -28712,7 +28715,7 @@
       </c>
     </row>
     <row r="31" spans="1:39" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="799"/>
+      <c r="A31" s="808"/>
       <c r="B31" s="126" t="s">
         <v>7</v>
       </c>
@@ -28743,7 +28746,7 @@
         <f>Indata!I$36</f>
         <v>10.009999999999998</v>
       </c>
-      <c r="K31" s="802"/>
+      <c r="K31" s="811"/>
       <c r="L31" s="661" t="s">
         <v>7</v>
       </c>
@@ -28774,7 +28777,7 @@
         <f>I31*(1-Indata!I$74)+I31*(1+Indata!I$76)*I$52</f>
         <v>10.009999999999998</v>
       </c>
-      <c r="U31" s="799"/>
+      <c r="U31" s="808"/>
       <c r="V31" s="126" t="s">
         <v>7</v>
       </c>
@@ -28805,7 +28808,7 @@
         <f t="shared" si="68"/>
         <v>10.009999999999998</v>
       </c>
-      <c r="AE31" s="799"/>
+      <c r="AE31" s="808"/>
       <c r="AF31" s="126" t="s">
         <v>7</v>
       </c>
@@ -29500,7 +29503,7 @@
       <c r="AM39" s="189"/>
     </row>
     <row r="40" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A40" s="797" t="s">
+      <c r="A40" s="806" t="s">
         <v>77</v>
       </c>
       <c r="B40" s="124" t="s">
@@ -29533,7 +29536,7 @@
         <f t="shared" si="84"/>
         <v>20.490767763608162</v>
       </c>
-      <c r="K40" s="797" t="s">
+      <c r="K40" s="806" t="s">
         <v>77</v>
       </c>
       <c r="L40" s="124" t="s">
@@ -29566,7 +29569,7 @@
         <f t="shared" si="85"/>
         <v>20.490767763608162</v>
       </c>
-      <c r="U40" s="797" t="s">
+      <c r="U40" s="806" t="s">
         <v>77</v>
       </c>
       <c r="V40" s="124" t="s">
@@ -29599,7 +29602,7 @@
         <f t="shared" ref="AC40:AC42" si="90">S40</f>
         <v>20.490767763608162</v>
       </c>
-      <c r="AE40" s="797" t="s">
+      <c r="AE40" s="806" t="s">
         <v>77</v>
       </c>
       <c r="AF40" s="124" t="s">
@@ -29634,7 +29637,7 @@
       </c>
     </row>
     <row r="41" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A41" s="798"/>
+      <c r="A41" s="807"/>
       <c r="B41" s="125" t="s">
         <v>9</v>
       </c>
@@ -29665,7 +29668,7 @@
         <f t="shared" si="84"/>
         <v>21.099103565816492</v>
       </c>
-      <c r="K41" s="798"/>
+      <c r="K41" s="807"/>
       <c r="L41" s="125" t="s">
         <v>9</v>
       </c>
@@ -29696,7 +29699,7 @@
         <f t="shared" si="85"/>
         <v>21.099103565816492</v>
       </c>
-      <c r="U41" s="798"/>
+      <c r="U41" s="807"/>
       <c r="V41" s="125" t="s">
         <v>9</v>
       </c>
@@ -29727,7 +29730,7 @@
         <f t="shared" si="90"/>
         <v>21.099103565816492</v>
       </c>
-      <c r="AE41" s="798"/>
+      <c r="AE41" s="807"/>
       <c r="AF41" s="125" t="s">
         <v>9</v>
       </c>
@@ -29760,7 +29763,7 @@
       </c>
     </row>
     <row r="42" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A42" s="798"/>
+      <c r="A42" s="807"/>
       <c r="B42" s="125" t="s">
         <v>7</v>
       </c>
@@ -29791,7 +29794,7 @@
         <f t="shared" si="84"/>
         <v>16.728198124999999</v>
       </c>
-      <c r="K42" s="798"/>
+      <c r="K42" s="807"/>
       <c r="L42" s="125" t="s">
         <v>7</v>
       </c>
@@ -29822,7 +29825,7 @@
         <f t="shared" si="85"/>
         <v>16.728198124999999</v>
       </c>
-      <c r="U42" s="798"/>
+      <c r="U42" s="807"/>
       <c r="V42" s="125" t="s">
         <v>7</v>
       </c>
@@ -29853,7 +29856,7 @@
         <f t="shared" si="90"/>
         <v>16.728198124999999</v>
       </c>
-      <c r="AE42" s="798"/>
+      <c r="AE42" s="807"/>
       <c r="AF42" s="125" t="s">
         <v>7</v>
       </c>
@@ -29886,7 +29889,7 @@
       </c>
     </row>
     <row r="43" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A43" s="798"/>
+      <c r="A43" s="807"/>
       <c r="B43" s="175" t="s">
         <v>76</v>
       </c>
@@ -29915,7 +29918,7 @@
         <f t="shared" si="98"/>
         <v>19.250316494987008</v>
       </c>
-      <c r="K43" s="798"/>
+      <c r="K43" s="807"/>
       <c r="L43" s="175" t="s">
         <v>76</v>
       </c>
@@ -29946,7 +29949,7 @@
         <f t="shared" ref="S43" si="99">SUMPRODUCT(S40:S42,S34:S36)/S37</f>
         <v>19.250316494987008</v>
       </c>
-      <c r="U43" s="798"/>
+      <c r="U43" s="807"/>
       <c r="V43" s="175" t="s">
         <v>76</v>
       </c>
@@ -29977,7 +29980,7 @@
         <f t="shared" si="100"/>
         <v>19.250316494987008</v>
       </c>
-      <c r="AE43" s="798"/>
+      <c r="AE43" s="807"/>
       <c r="AF43" s="175" t="s">
         <v>76</v>
       </c>
@@ -30010,7 +30013,7 @@
       </c>
     </row>
     <row r="44" spans="1:39" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="799"/>
+      <c r="A44" s="808"/>
       <c r="B44" s="176" t="s">
         <v>229</v>
       </c>
@@ -30035,7 +30038,7 @@
       <c r="I44" s="213" t="s">
         <v>78</v>
       </c>
-      <c r="K44" s="799"/>
+      <c r="K44" s="808"/>
       <c r="L44" s="176" t="s">
         <v>229</v>
       </c>
@@ -30066,7 +30069,7 @@
         <f>S43/E43-1</f>
         <v>-2.0590298791616446E-2</v>
       </c>
-      <c r="U44" s="799"/>
+      <c r="U44" s="808"/>
       <c r="V44" s="176" t="s">
         <v>229</v>
       </c>
@@ -30097,7 +30100,7 @@
         <f>AC43/E43-1</f>
         <v>-2.0590298791616446E-2</v>
       </c>
-      <c r="AE44" s="799"/>
+      <c r="AE44" s="808"/>
       <c r="AF44" s="176" t="s">
         <v>229</v>
       </c>
@@ -30205,7 +30208,7 @@
       <c r="AM46" s="75"/>
     </row>
     <row r="47" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A47" s="800" t="s">
+      <c r="A47" s="809" t="s">
         <v>29</v>
       </c>
       <c r="B47" s="659" t="s">
@@ -30238,7 +30241,7 @@
         <f>Indata!I39</f>
         <v>11648700</v>
       </c>
-      <c r="K47" s="800" t="s">
+      <c r="K47" s="809" t="s">
         <v>29</v>
       </c>
       <c r="L47" s="659" t="s">
@@ -30271,7 +30274,7 @@
         <f t="shared" si="101"/>
         <v>11648700</v>
       </c>
-      <c r="U47" s="797" t="s">
+      <c r="U47" s="806" t="s">
         <v>29</v>
       </c>
       <c r="V47" s="124" t="s">
@@ -30304,7 +30307,7 @@
         <f t="shared" ref="AC47:AC49" si="106">S47</f>
         <v>11648700</v>
       </c>
-      <c r="AE47" s="797" t="s">
+      <c r="AE47" s="806" t="s">
         <v>29</v>
       </c>
       <c r="AF47" s="124" t="s">
@@ -30339,7 +30342,7 @@
       </c>
     </row>
     <row r="48" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A48" s="801"/>
+      <c r="A48" s="810"/>
       <c r="B48" s="660" t="s">
         <v>645</v>
       </c>
@@ -30370,7 +30373,7 @@
         <f>Indata!I40</f>
         <v>0.52928701904391762</v>
       </c>
-      <c r="K48" s="801"/>
+      <c r="K48" s="810"/>
       <c r="L48" s="660" t="s">
         <v>646</v>
       </c>
@@ -30401,7 +30404,7 @@
         <f>(1+'Indata - Effektsamband-Faktorer'!$D$7*S44)*I51</f>
         <v>0.53037683683078141</v>
       </c>
-      <c r="U48" s="798"/>
+      <c r="U48" s="807"/>
       <c r="V48" s="125" t="s">
         <v>29</v>
       </c>
@@ -30432,7 +30435,7 @@
         <f t="shared" si="106"/>
         <v>0.53037683683078141</v>
       </c>
-      <c r="AE48" s="798"/>
+      <c r="AE48" s="807"/>
       <c r="AF48" s="125" t="s">
         <v>29</v>
       </c>
@@ -30465,7 +30468,7 @@
       </c>
     </row>
     <row r="49" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A49" s="801"/>
+      <c r="A49" s="810"/>
       <c r="B49" s="660" t="s">
         <v>647</v>
       </c>
@@ -30496,7 +30499,7 @@
         <f t="shared" si="112"/>
         <v>6165505.6987368828</v>
       </c>
-      <c r="K49" s="801"/>
+      <c r="K49" s="810"/>
       <c r="L49" s="660" t="s">
         <v>644</v>
       </c>
@@ -30527,7 +30530,7 @@
         <f t="shared" si="113"/>
         <v>6178200.6591907237</v>
       </c>
-      <c r="U49" s="798"/>
+      <c r="U49" s="807"/>
       <c r="V49" s="125" t="s">
         <v>34</v>
       </c>
@@ -30558,7 +30561,7 @@
         <f t="shared" si="106"/>
         <v>6178200.6591907237</v>
       </c>
-      <c r="AE49" s="798"/>
+      <c r="AE49" s="807"/>
       <c r="AF49" s="125" t="s">
         <v>34</v>
       </c>
@@ -30591,7 +30594,7 @@
       </c>
     </row>
     <row r="50" spans="1:39" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="801"/>
+      <c r="A50" s="810"/>
       <c r="B50" s="660" t="s">
         <v>644</v>
       </c>
@@ -30622,7 +30625,7 @@
         <f>I49*Indata!I$74*Indata!I$77+I49*(1-Indata!I$74)</f>
         <v>6165505.6987368828</v>
       </c>
-      <c r="K50" s="802"/>
+      <c r="K50" s="811"/>
       <c r="L50" s="661" t="s">
         <v>229</v>
       </c>
@@ -30653,7 +30656,7 @@
         <f>S49/E50-1</f>
         <v>2.0590298791616224E-3</v>
       </c>
-      <c r="U50" s="799"/>
+      <c r="U50" s="808"/>
       <c r="V50" s="126" t="s">
         <v>229</v>
       </c>
@@ -30684,7 +30687,7 @@
         <f>AC49/E49-1</f>
         <v>2.0590298791616224E-3</v>
       </c>
-      <c r="AE50" s="799"/>
+      <c r="AE50" s="808"/>
       <c r="AF50" s="126" t="s">
         <v>229</v>
       </c>
@@ -32295,6 +32298,48 @@
     </row>
   </sheetData>
   <mergeCells count="58">
+    <mergeCell ref="AE57:AE60"/>
+    <mergeCell ref="AE61:AE64"/>
+    <mergeCell ref="A18:A21"/>
+    <mergeCell ref="K18:K21"/>
+    <mergeCell ref="A34:A37"/>
+    <mergeCell ref="U18:U21"/>
+    <mergeCell ref="U24:U26"/>
+    <mergeCell ref="U29:U31"/>
+    <mergeCell ref="U34:U37"/>
+    <mergeCell ref="U40:U44"/>
+    <mergeCell ref="U47:U50"/>
+    <mergeCell ref="AE34:AE37"/>
+    <mergeCell ref="AE40:AE44"/>
+    <mergeCell ref="A13:A15"/>
+    <mergeCell ref="K47:K50"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="K6:K10"/>
+    <mergeCell ref="A40:A44"/>
+    <mergeCell ref="K40:K44"/>
+    <mergeCell ref="A6:A10"/>
+    <mergeCell ref="A47:A50"/>
+    <mergeCell ref="A24:A26"/>
+    <mergeCell ref="A29:A31"/>
+    <mergeCell ref="K34:K37"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="K24:K26"/>
+    <mergeCell ref="K29:K31"/>
+    <mergeCell ref="K13:K15"/>
+    <mergeCell ref="Z3:AA3"/>
+    <mergeCell ref="AB3:AC3"/>
+    <mergeCell ref="U6:U10"/>
+    <mergeCell ref="U13:U15"/>
+    <mergeCell ref="N3:O3"/>
+    <mergeCell ref="P3:Q3"/>
+    <mergeCell ref="R3:S3"/>
+    <mergeCell ref="AH3:AI3"/>
+    <mergeCell ref="AJ3:AK3"/>
+    <mergeCell ref="AL3:AM3"/>
+    <mergeCell ref="AE6:AE10"/>
+    <mergeCell ref="AE13:AE15"/>
+    <mergeCell ref="AF3:AG4"/>
     <mergeCell ref="AE86:AE89"/>
     <mergeCell ref="A3:A4"/>
     <mergeCell ref="B3:C4"/>
@@ -32311,48 +32356,6 @@
     <mergeCell ref="AE24:AE26"/>
     <mergeCell ref="AE29:AE31"/>
     <mergeCell ref="X3:Y3"/>
-    <mergeCell ref="AH3:AI3"/>
-    <mergeCell ref="AJ3:AK3"/>
-    <mergeCell ref="AL3:AM3"/>
-    <mergeCell ref="AE6:AE10"/>
-    <mergeCell ref="AE13:AE15"/>
-    <mergeCell ref="AF3:AG4"/>
-    <mergeCell ref="Z3:AA3"/>
-    <mergeCell ref="AB3:AC3"/>
-    <mergeCell ref="U6:U10"/>
-    <mergeCell ref="U13:U15"/>
-    <mergeCell ref="N3:O3"/>
-    <mergeCell ref="P3:Q3"/>
-    <mergeCell ref="R3:S3"/>
-    <mergeCell ref="A13:A15"/>
-    <mergeCell ref="K47:K50"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="K6:K10"/>
-    <mergeCell ref="A40:A44"/>
-    <mergeCell ref="K40:K44"/>
-    <mergeCell ref="A6:A10"/>
-    <mergeCell ref="A47:A50"/>
-    <mergeCell ref="A24:A26"/>
-    <mergeCell ref="A29:A31"/>
-    <mergeCell ref="K34:K37"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="K24:K26"/>
-    <mergeCell ref="K29:K31"/>
-    <mergeCell ref="K13:K15"/>
-    <mergeCell ref="AE57:AE60"/>
-    <mergeCell ref="AE61:AE64"/>
-    <mergeCell ref="A18:A21"/>
-    <mergeCell ref="K18:K21"/>
-    <mergeCell ref="A34:A37"/>
-    <mergeCell ref="U18:U21"/>
-    <mergeCell ref="U24:U26"/>
-    <mergeCell ref="U29:U31"/>
-    <mergeCell ref="U34:U37"/>
-    <mergeCell ref="U40:U44"/>
-    <mergeCell ref="U47:U50"/>
-    <mergeCell ref="AE34:AE37"/>
-    <mergeCell ref="AE40:AE44"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -32367,9 +32370,9 @@
   </sheetPr>
   <dimension ref="A1:AM114"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A60" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AH89" sqref="AH89"/>
+    <sheetView zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
+      <pane ySplit="4" topLeftCell="A46" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G45" sqref="G45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -32406,10 +32409,10 @@
       <c r="A3" s="791" t="s">
         <v>67</v>
       </c>
-      <c r="B3" s="808" t="s">
+      <c r="B3" s="798" t="s">
         <v>222</v>
       </c>
-      <c r="C3" s="809"/>
+      <c r="C3" s="799"/>
       <c r="D3" s="791" t="s">
         <v>64</v>
       </c>
@@ -32425,10 +32428,10 @@
       <c r="K3" s="791" t="s">
         <v>67</v>
       </c>
-      <c r="L3" s="808" t="s">
+      <c r="L3" s="798" t="s">
         <v>235</v>
       </c>
-      <c r="M3" s="809"/>
+      <c r="M3" s="799"/>
       <c r="N3" s="791" t="s">
         <v>64</v>
       </c>
@@ -32444,10 +32447,10 @@
       <c r="U3" s="791" t="s">
         <v>67</v>
       </c>
-      <c r="V3" s="808" t="s">
+      <c r="V3" s="798" t="s">
         <v>236</v>
       </c>
-      <c r="W3" s="809"/>
+      <c r="W3" s="799"/>
       <c r="X3" s="791" t="s">
         <v>64</v>
       </c>
@@ -32463,10 +32466,10 @@
       <c r="AE3" s="791" t="s">
         <v>67</v>
       </c>
-      <c r="AF3" s="808" t="s">
+      <c r="AF3" s="798" t="s">
         <v>233</v>
       </c>
-      <c r="AG3" s="809"/>
+      <c r="AG3" s="799"/>
       <c r="AH3" s="791" t="s">
         <v>64</v>
       </c>
@@ -32481,9 +32484,9 @@
       <c r="AM3" s="792"/>
     </row>
     <row r="4" spans="1:39" s="118" customFormat="1" ht="41.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="807"/>
-      <c r="B4" s="810"/>
-      <c r="C4" s="811"/>
+      <c r="A4" s="797"/>
+      <c r="B4" s="800"/>
+      <c r="C4" s="801"/>
       <c r="D4" s="253">
         <v>2030</v>
       </c>
@@ -32502,9 +32505,9 @@
       <c r="I4" s="254">
         <v>2040</v>
       </c>
-      <c r="K4" s="807"/>
-      <c r="L4" s="810"/>
-      <c r="M4" s="811"/>
+      <c r="K4" s="797"/>
+      <c r="L4" s="800"/>
+      <c r="M4" s="801"/>
       <c r="N4" s="253">
         <v>2030</v>
       </c>
@@ -32523,9 +32526,9 @@
       <c r="S4" s="254">
         <v>2040</v>
       </c>
-      <c r="U4" s="807"/>
-      <c r="V4" s="810"/>
-      <c r="W4" s="811"/>
+      <c r="U4" s="797"/>
+      <c r="V4" s="800"/>
+      <c r="W4" s="801"/>
       <c r="X4" s="253">
         <v>2030</v>
       </c>
@@ -32544,9 +32547,9 @@
       <c r="AC4" s="254">
         <v>2040</v>
       </c>
-      <c r="AE4" s="807"/>
-      <c r="AF4" s="810"/>
-      <c r="AG4" s="811"/>
+      <c r="AE4" s="797"/>
+      <c r="AF4" s="800"/>
+      <c r="AG4" s="801"/>
       <c r="AH4" s="253">
         <v>2030</v>
       </c>
@@ -32607,7 +32610,7 @@
       <c r="AM5" s="73"/>
     </row>
     <row r="6" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A6" s="797" t="s">
+      <c r="A6" s="806" t="s">
         <v>0</v>
       </c>
       <c r="B6" s="124" t="s">
@@ -32640,7 +32643,7 @@
         <f>Indata!I58</f>
         <v>16.350158148247193</v>
       </c>
-      <c r="K6" s="797" t="s">
+      <c r="K6" s="806" t="s">
         <v>0</v>
       </c>
       <c r="L6" s="124" t="s">
@@ -32673,7 +32676,7 @@
         <f>'Modell - Drivmedelpriser'!J58</f>
         <v>16.350158148247193</v>
       </c>
-      <c r="U6" s="797" t="s">
+      <c r="U6" s="806" t="s">
         <v>0</v>
       </c>
       <c r="V6" s="124" t="s">
@@ -32706,7 +32709,7 @@
         <f t="shared" si="0"/>
         <v>16.350158148247193</v>
       </c>
-      <c r="AE6" s="797" t="s">
+      <c r="AE6" s="806" t="s">
         <v>0</v>
       </c>
       <c r="AF6" s="124" t="s">
@@ -32741,7 +32744,7 @@
       </c>
     </row>
     <row r="7" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A7" s="798"/>
+      <c r="A7" s="807"/>
       <c r="B7" s="125" t="s">
         <v>7</v>
       </c>
@@ -32772,7 +32775,7 @@
         <f>Indata!I59</f>
         <v>1.4034</v>
       </c>
-      <c r="K7" s="798"/>
+      <c r="K7" s="807"/>
       <c r="L7" s="125" t="s">
         <v>7</v>
       </c>
@@ -32803,7 +32806,7 @@
         <f>'Modell - Drivmedelpriser'!J84</f>
         <v>1.4034</v>
       </c>
-      <c r="U7" s="798"/>
+      <c r="U7" s="807"/>
       <c r="V7" s="125" t="s">
         <v>7</v>
       </c>
@@ -32834,7 +32837,7 @@
         <f t="shared" si="0"/>
         <v>1.4034</v>
       </c>
-      <c r="AE7" s="798"/>
+      <c r="AE7" s="807"/>
       <c r="AF7" s="125" t="s">
         <v>7</v>
       </c>
@@ -32867,7 +32870,7 @@
       </c>
     </row>
     <row r="8" spans="1:39" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="799"/>
+      <c r="A8" s="808"/>
       <c r="B8" s="176" t="s">
         <v>239</v>
       </c>
@@ -32892,7 +32895,7 @@
       <c r="I8" s="275" t="s">
         <v>78</v>
       </c>
-      <c r="K8" s="799"/>
+      <c r="K8" s="808"/>
       <c r="L8" s="176" t="s">
         <v>239</v>
       </c>
@@ -32923,7 +32926,7 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="U8" s="799"/>
+      <c r="U8" s="808"/>
       <c r="V8" s="176" t="s">
         <v>239</v>
       </c>
@@ -32954,7 +32957,7 @@
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="AE8" s="799"/>
+      <c r="AE8" s="808"/>
       <c r="AF8" s="176" t="s">
         <v>239</v>
       </c>
@@ -34965,7 +34968,7 @@
       <c r="AM28" s="74"/>
     </row>
     <row r="29" spans="1:39" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="797" t="s">
+      <c r="A29" s="806" t="s">
         <v>21</v>
       </c>
       <c r="B29" s="124" t="s">
@@ -34998,7 +35001,7 @@
         <f>Indata!I$16*10</f>
         <v>0</v>
       </c>
-      <c r="K29" s="797" t="s">
+      <c r="K29" s="806" t="s">
         <v>21</v>
       </c>
       <c r="L29" s="124" t="s">
@@ -35031,7 +35034,7 @@
         <f t="shared" ref="S29:S32" si="43">I29</f>
         <v>0</v>
       </c>
-      <c r="U29" s="797" t="s">
+      <c r="U29" s="806" t="s">
         <v>21</v>
       </c>
       <c r="V29" s="124" t="s">
@@ -35064,7 +35067,7 @@
         <f t="shared" si="44"/>
         <v>0</v>
       </c>
-      <c r="AE29" s="797" t="s">
+      <c r="AE29" s="806" t="s">
         <v>21</v>
       </c>
       <c r="AF29" s="124" t="s">
@@ -35099,7 +35102,7 @@
       </c>
     </row>
     <row r="30" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A30" s="798"/>
+      <c r="A30" s="807"/>
       <c r="B30" s="125" t="s">
         <v>116</v>
       </c>
@@ -35130,7 +35133,7 @@
         <f>Indata!I$16*10</f>
         <v>0</v>
       </c>
-      <c r="K30" s="798"/>
+      <c r="K30" s="807"/>
       <c r="L30" s="125" t="s">
         <v>116</v>
       </c>
@@ -35161,7 +35164,7 @@
         <f t="shared" si="43"/>
         <v>0</v>
       </c>
-      <c r="U30" s="798"/>
+      <c r="U30" s="807"/>
       <c r="V30" s="125" t="s">
         <v>116</v>
       </c>
@@ -35192,7 +35195,7 @@
         <f t="shared" si="44"/>
         <v>0</v>
       </c>
-      <c r="AE30" s="798"/>
+      <c r="AE30" s="807"/>
       <c r="AF30" s="125" t="s">
         <v>116</v>
       </c>
@@ -35225,7 +35228,7 @@
       </c>
     </row>
     <row r="31" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A31" s="798"/>
+      <c r="A31" s="807"/>
       <c r="B31" s="125" t="s">
         <v>117</v>
       </c>
@@ -35256,7 +35259,7 @@
         <f>Indata!I$16*10</f>
         <v>0</v>
       </c>
-      <c r="K31" s="798"/>
+      <c r="K31" s="807"/>
       <c r="L31" s="125" t="s">
         <v>117</v>
       </c>
@@ -35287,7 +35290,7 @@
         <f t="shared" si="43"/>
         <v>0</v>
       </c>
-      <c r="U31" s="798"/>
+      <c r="U31" s="807"/>
       <c r="V31" s="125" t="s">
         <v>117</v>
       </c>
@@ -35318,7 +35321,7 @@
         <f t="shared" si="44"/>
         <v>0</v>
       </c>
-      <c r="AE31" s="798"/>
+      <c r="AE31" s="807"/>
       <c r="AF31" s="125" t="s">
         <v>117</v>
       </c>
@@ -35351,7 +35354,7 @@
       </c>
     </row>
     <row r="32" spans="1:39" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="799"/>
+      <c r="A32" s="808"/>
       <c r="B32" s="126" t="s">
         <v>118</v>
       </c>
@@ -35382,7 +35385,7 @@
         <f>Indata!I$16*10</f>
         <v>0</v>
       </c>
-      <c r="K32" s="799"/>
+      <c r="K32" s="808"/>
       <c r="L32" s="126" t="s">
         <v>118</v>
       </c>
@@ -35413,7 +35416,7 @@
         <f t="shared" si="43"/>
         <v>0</v>
       </c>
-      <c r="U32" s="799"/>
+      <c r="U32" s="808"/>
       <c r="V32" s="126" t="s">
         <v>118</v>
       </c>
@@ -35444,7 +35447,7 @@
         <f t="shared" si="44"/>
         <v>0</v>
       </c>
-      <c r="AE32" s="799"/>
+      <c r="AE32" s="808"/>
       <c r="AF32" s="126" t="s">
         <v>118</v>
       </c>
@@ -42405,6 +42408,44 @@
     </row>
   </sheetData>
   <mergeCells count="54">
+    <mergeCell ref="U23:U26"/>
+    <mergeCell ref="AE23:AE26"/>
+    <mergeCell ref="U6:U8"/>
+    <mergeCell ref="AE106:AE109"/>
+    <mergeCell ref="AE92:AE94"/>
+    <mergeCell ref="AE95:AE97"/>
+    <mergeCell ref="U53:U68"/>
+    <mergeCell ref="AE53:AE68"/>
+    <mergeCell ref="AE6:AE8"/>
+    <mergeCell ref="A11:A20"/>
+    <mergeCell ref="K11:K20"/>
+    <mergeCell ref="AE89:AE91"/>
+    <mergeCell ref="AE101:AE103"/>
+    <mergeCell ref="A36:A50"/>
+    <mergeCell ref="K36:K50"/>
+    <mergeCell ref="U36:U50"/>
+    <mergeCell ref="AE36:AE50"/>
+    <mergeCell ref="A29:A32"/>
+    <mergeCell ref="K29:K32"/>
+    <mergeCell ref="U11:U20"/>
+    <mergeCell ref="AE11:AE20"/>
+    <mergeCell ref="U29:U32"/>
+    <mergeCell ref="A53:A68"/>
+    <mergeCell ref="K53:K68"/>
+    <mergeCell ref="AE29:AE32"/>
+    <mergeCell ref="AL3:AM3"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="N3:O3"/>
+    <mergeCell ref="P3:Q3"/>
+    <mergeCell ref="R3:S3"/>
+    <mergeCell ref="AF3:AG4"/>
+    <mergeCell ref="X3:Y3"/>
+    <mergeCell ref="Z3:AA3"/>
+    <mergeCell ref="AB3:AC3"/>
+    <mergeCell ref="AH3:AI3"/>
+    <mergeCell ref="AJ3:AK3"/>
     <mergeCell ref="AE110:AE114"/>
     <mergeCell ref="A3:A4"/>
     <mergeCell ref="B3:C4"/>
@@ -42421,44 +42462,6 @@
     <mergeCell ref="K6:K8"/>
     <mergeCell ref="A23:A26"/>
     <mergeCell ref="K23:K26"/>
-    <mergeCell ref="AL3:AM3"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="N3:O3"/>
-    <mergeCell ref="P3:Q3"/>
-    <mergeCell ref="R3:S3"/>
-    <mergeCell ref="AF3:AG4"/>
-    <mergeCell ref="X3:Y3"/>
-    <mergeCell ref="Z3:AA3"/>
-    <mergeCell ref="AB3:AC3"/>
-    <mergeCell ref="AH3:AI3"/>
-    <mergeCell ref="AJ3:AK3"/>
-    <mergeCell ref="A11:A20"/>
-    <mergeCell ref="K11:K20"/>
-    <mergeCell ref="AE89:AE91"/>
-    <mergeCell ref="AE101:AE103"/>
-    <mergeCell ref="A36:A50"/>
-    <mergeCell ref="K36:K50"/>
-    <mergeCell ref="U36:U50"/>
-    <mergeCell ref="AE36:AE50"/>
-    <mergeCell ref="A29:A32"/>
-    <mergeCell ref="K29:K32"/>
-    <mergeCell ref="U11:U20"/>
-    <mergeCell ref="AE11:AE20"/>
-    <mergeCell ref="U29:U32"/>
-    <mergeCell ref="A53:A68"/>
-    <mergeCell ref="K53:K68"/>
-    <mergeCell ref="AE29:AE32"/>
-    <mergeCell ref="U23:U26"/>
-    <mergeCell ref="AE23:AE26"/>
-    <mergeCell ref="U6:U8"/>
-    <mergeCell ref="AE106:AE109"/>
-    <mergeCell ref="AE92:AE94"/>
-    <mergeCell ref="AE95:AE97"/>
-    <mergeCell ref="U53:U68"/>
-    <mergeCell ref="AE53:AE68"/>
-    <mergeCell ref="AE6:AE8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -42559,18 +42562,18 @@
       <c r="C4" s="121" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="785" t="s">
+      <c r="D4" s="775" t="s">
         <v>64</v>
       </c>
-      <c r="E4" s="786"/>
-      <c r="F4" s="785" t="s">
+      <c r="E4" s="776"/>
+      <c r="F4" s="775" t="s">
         <v>65</v>
       </c>
-      <c r="G4" s="786"/>
-      <c r="H4" s="785" t="s">
+      <c r="G4" s="776"/>
+      <c r="H4" s="775" t="s">
         <v>66</v>
       </c>
-      <c r="I4" s="786"/>
+      <c r="I4" s="776"/>
       <c r="J4" s="38"/>
       <c r="K4" s="38"/>
       <c r="L4" s="38"/>
@@ -42586,21 +42589,21 @@
       </c>
       <c r="B5" s="278"/>
       <c r="C5" s="279"/>
-      <c r="D5" s="818" t="str">
+      <c r="D5" s="832" t="str">
         <f>Indata!D6</f>
         <v>Beslutad politik - Trafikverkets basscenario, ändras ej av EMA!</v>
       </c>
-      <c r="E5" s="819"/>
-      <c r="F5" s="818" t="str">
+      <c r="E5" s="833"/>
+      <c r="F5" s="832" t="str">
         <f>Indata!F6</f>
         <v>Policy scenario (EMA)</v>
       </c>
-      <c r="G5" s="819"/>
-      <c r="H5" s="818" t="str">
+      <c r="G5" s="833"/>
+      <c r="H5" s="832" t="str">
         <f>Indata!H6</f>
         <v>Reference scenario (EMA -beslutad politik, varierande X)</v>
       </c>
-      <c r="I5" s="819"/>
+      <c r="I5" s="833"/>
       <c r="J5" s="63"/>
       <c r="K5" s="63"/>
       <c r="L5" s="63"/>
@@ -42648,7 +42651,7 @@
       <c r="Q6" s="118"/>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A7" s="820" t="s">
+      <c r="A7" s="829" t="s">
         <v>0</v>
       </c>
       <c r="B7" s="280" t="s">
@@ -42683,7 +42686,7 @@
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A8" s="822"/>
+      <c r="A8" s="830"/>
       <c r="B8" s="75" t="s">
         <v>102</v>
       </c>
@@ -42716,7 +42719,7 @@
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A9" s="822"/>
+      <c r="A9" s="830"/>
       <c r="B9" s="75" t="s">
         <v>103</v>
       </c>
@@ -42749,7 +42752,7 @@
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A10" s="822"/>
+      <c r="A10" s="830"/>
       <c r="B10" s="75" t="s">
         <v>180</v>
       </c>
@@ -42782,7 +42785,7 @@
       </c>
     </row>
     <row r="11" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="821"/>
+      <c r="A11" s="831"/>
       <c r="B11" s="281" t="s">
         <v>181</v>
       </c>
@@ -42815,7 +42818,7 @@
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A12" s="820" t="s">
+      <c r="A12" s="829" t="s">
         <v>38</v>
       </c>
       <c r="B12" s="280" t="s">
@@ -42850,7 +42853,7 @@
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A13" s="822"/>
+      <c r="A13" s="830"/>
       <c r="B13" s="75" t="s">
         <v>102</v>
       </c>
@@ -42883,7 +42886,7 @@
       </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A14" s="822"/>
+      <c r="A14" s="830"/>
       <c r="B14" s="75" t="s">
         <v>103</v>
       </c>
@@ -42916,7 +42919,7 @@
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A15" s="822"/>
+      <c r="A15" s="830"/>
       <c r="B15" s="75" t="s">
         <v>352</v>
       </c>
@@ -42949,7 +42952,7 @@
       </c>
     </row>
     <row r="16" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="821"/>
+      <c r="A16" s="831"/>
       <c r="B16" s="281" t="s">
         <v>318</v>
       </c>
@@ -42982,7 +42985,7 @@
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" s="820" t="s">
+      <c r="A17" s="829" t="s">
         <v>21</v>
       </c>
       <c r="B17" s="280" t="s">
@@ -43017,7 +43020,7 @@
       </c>
     </row>
     <row r="18" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="821"/>
+      <c r="A18" s="831"/>
       <c r="B18" s="281" t="s">
         <v>319</v>
       </c>
@@ -43085,7 +43088,7 @@
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20" s="820" t="s">
+      <c r="A20" s="829" t="s">
         <v>77</v>
       </c>
       <c r="B20" s="280" t="s">
@@ -43122,7 +43125,7 @@
       <c r="K20" s="403"/>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A21" s="822"/>
+      <c r="A21" s="830"/>
       <c r="B21" s="75" t="s">
         <v>102</v>
       </c>
@@ -43155,7 +43158,7 @@
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A22" s="822"/>
+      <c r="A22" s="830"/>
       <c r="B22" s="75" t="s">
         <v>103</v>
       </c>
@@ -43188,7 +43191,7 @@
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A23" s="822"/>
+      <c r="A23" s="830"/>
       <c r="B23" s="370" t="s">
         <v>179</v>
       </c>
@@ -43221,7 +43224,7 @@
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A24" s="822"/>
+      <c r="A24" s="830"/>
       <c r="B24" s="75" t="s">
         <v>352</v>
       </c>
@@ -43254,7 +43257,7 @@
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A25" s="822"/>
+      <c r="A25" s="830"/>
       <c r="B25" s="75" t="s">
         <v>318</v>
       </c>
@@ -43287,7 +43290,7 @@
       </c>
     </row>
     <row r="26" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="821"/>
+      <c r="A26" s="831"/>
       <c r="B26" s="371" t="s">
         <v>353</v>
       </c>
@@ -43320,7 +43323,7 @@
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A27" s="820" t="s">
+      <c r="A27" s="829" t="s">
         <v>17</v>
       </c>
       <c r="B27" s="280" t="s">
@@ -43355,7 +43358,7 @@
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A28" s="822"/>
+      <c r="A28" s="830"/>
       <c r="B28" s="75" t="s">
         <v>102</v>
       </c>
@@ -43388,7 +43391,7 @@
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A29" s="822"/>
+      <c r="A29" s="830"/>
       <c r="B29" s="75" t="s">
         <v>103</v>
       </c>
@@ -43421,7 +43424,7 @@
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A30" s="822"/>
+      <c r="A30" s="830"/>
       <c r="B30" s="370" t="s">
         <v>104</v>
       </c>
@@ -43454,7 +43457,7 @@
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A31" s="822"/>
+      <c r="A31" s="830"/>
       <c r="B31" s="75" t="s">
         <v>354</v>
       </c>
@@ -43487,7 +43490,7 @@
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A32" s="822"/>
+      <c r="A32" s="830"/>
       <c r="B32" s="75" t="s">
         <v>318</v>
       </c>
@@ -43520,7 +43523,7 @@
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A33" s="822"/>
+      <c r="A33" s="830"/>
       <c r="B33" s="370" t="s">
         <v>355</v>
       </c>
@@ -43553,7 +43556,7 @@
       </c>
     </row>
     <row r="34" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="821"/>
+      <c r="A34" s="831"/>
       <c r="B34" s="371" t="s">
         <v>332</v>
       </c>
@@ -43586,7 +43589,7 @@
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A35" s="822" t="s">
+      <c r="A35" s="830" t="s">
         <v>285</v>
       </c>
       <c r="B35" s="75" t="s">
@@ -43621,7 +43624,7 @@
       </c>
     </row>
     <row r="36" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="821"/>
+      <c r="A36" s="831"/>
       <c r="B36" s="281" t="s">
         <v>319</v>
       </c>
@@ -43654,7 +43657,7 @@
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A37" s="823" t="s">
+      <c r="A37" s="827" t="s">
         <v>274</v>
       </c>
       <c r="B37" s="280" t="s">
@@ -43689,7 +43692,7 @@
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A38" s="824"/>
+      <c r="A38" s="828"/>
       <c r="B38" s="75" t="s">
         <v>319</v>
       </c>
@@ -43722,7 +43725,7 @@
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A39" s="824"/>
+      <c r="A39" s="828"/>
       <c r="B39" s="75" t="s">
         <v>310</v>
       </c>
@@ -43749,7 +43752,7 @@
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A40" s="824"/>
+      <c r="A40" s="828"/>
       <c r="B40" s="370" t="s">
         <v>16</v>
       </c>
@@ -43782,7 +43785,7 @@
       </c>
     </row>
     <row r="41" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="824"/>
+      <c r="A41" s="828"/>
       <c r="B41" s="492" t="s">
         <v>356</v>
       </c>
@@ -43815,7 +43818,7 @@
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A42" s="820" t="s">
+      <c r="A42" s="829" t="s">
         <v>271</v>
       </c>
       <c r="B42" s="280" t="s">
@@ -43850,7 +43853,7 @@
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A43" s="822"/>
+      <c r="A43" s="830"/>
       <c r="B43" s="75" t="s">
         <v>319</v>
       </c>
@@ -43883,7 +43886,7 @@
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A44" s="822"/>
+      <c r="A44" s="830"/>
       <c r="B44" s="370" t="s">
         <v>16</v>
       </c>
@@ -43949,7 +43952,7 @@
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A46" s="822" t="s">
+      <c r="A46" s="830" t="s">
         <v>265</v>
       </c>
       <c r="B46" s="75" t="s">
@@ -43984,7 +43987,7 @@
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A47" s="822"/>
+      <c r="A47" s="830"/>
       <c r="B47" s="75" t="s">
         <v>319</v>
       </c>
@@ -44017,7 +44020,7 @@
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A48" s="822"/>
+      <c r="A48" s="830"/>
       <c r="B48" s="370" t="s">
         <v>16</v>
       </c>
@@ -44081,7 +44084,7 @@
       </c>
     </row>
     <row r="50" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A50" s="820" t="s">
+      <c r="A50" s="829" t="s">
         <v>266</v>
       </c>
       <c r="B50" s="280" t="s">
@@ -44116,7 +44119,7 @@
       </c>
     </row>
     <row r="51" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A51" s="822"/>
+      <c r="A51" s="830"/>
       <c r="B51" s="75" t="s">
         <v>319</v>
       </c>
@@ -44149,7 +44152,7 @@
       </c>
     </row>
     <row r="52" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A52" s="822"/>
+      <c r="A52" s="830"/>
       <c r="B52" s="370" t="s">
         <v>16</v>
       </c>
@@ -44213,7 +44216,7 @@
       </c>
     </row>
     <row r="54" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A54" s="825" t="s">
+      <c r="A54" s="824" t="s">
         <v>129</v>
       </c>
       <c r="B54" s="280" t="s">
@@ -44248,7 +44251,7 @@
       </c>
     </row>
     <row r="55" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A55" s="826"/>
+      <c r="A55" s="825"/>
       <c r="B55" s="75" t="s">
         <v>315</v>
       </c>
@@ -44281,7 +44284,7 @@
       </c>
     </row>
     <row r="56" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A56" s="826"/>
+      <c r="A56" s="825"/>
       <c r="B56" s="75" t="s">
         <v>103</v>
       </c>
@@ -44314,7 +44317,7 @@
       </c>
     </row>
     <row r="57" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A57" s="826"/>
+      <c r="A57" s="825"/>
       <c r="B57" s="75" t="s">
         <v>312</v>
       </c>
@@ -44351,7 +44354,7 @@
       <c r="O57" s="495"/>
     </row>
     <row r="58" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A58" s="826"/>
+      <c r="A58" s="825"/>
       <c r="B58" s="75" t="s">
         <v>313</v>
       </c>
@@ -44384,7 +44387,7 @@
       </c>
     </row>
     <row r="59" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A59" s="826"/>
+      <c r="A59" s="825"/>
       <c r="B59" s="75" t="s">
         <v>314</v>
       </c>
@@ -44417,7 +44420,7 @@
       </c>
     </row>
     <row r="60" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A60" s="826"/>
+      <c r="A60" s="825"/>
       <c r="B60" s="370" t="s">
         <v>194</v>
       </c>
@@ -44454,7 +44457,7 @@
       <c r="O60" s="495"/>
     </row>
     <row r="61" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A61" s="826"/>
+      <c r="A61" s="825"/>
       <c r="B61" s="370" t="s">
         <v>195</v>
       </c>
@@ -44487,7 +44490,7 @@
       </c>
     </row>
     <row r="62" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A62" s="826"/>
+      <c r="A62" s="825"/>
       <c r="B62" s="370" t="s">
         <v>196</v>
       </c>
@@ -44520,7 +44523,7 @@
       </c>
     </row>
     <row r="63" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A63" s="827"/>
+      <c r="A63" s="826"/>
       <c r="B63" s="371" t="s">
         <v>358</v>
       </c>
@@ -44553,7 +44556,7 @@
       </c>
     </row>
     <row r="64" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A64" s="826" t="s">
+      <c r="A64" s="825" t="s">
         <v>240</v>
       </c>
       <c r="B64" s="75" t="s">
@@ -44588,7 +44591,7 @@
       </c>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A65" s="826"/>
+      <c r="A65" s="825"/>
       <c r="B65" s="75" t="s">
         <v>193</v>
       </c>
@@ -44621,7 +44624,7 @@
       </c>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A66" s="826"/>
+      <c r="A66" s="825"/>
       <c r="B66" s="75" t="s">
         <v>103</v>
       </c>
@@ -44654,7 +44657,7 @@
       </c>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A67" s="826"/>
+      <c r="A67" s="825"/>
       <c r="B67" s="75" t="s">
         <v>317</v>
       </c>
@@ -44687,7 +44690,7 @@
       </c>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A68" s="826"/>
+      <c r="A68" s="825"/>
       <c r="B68" s="75" t="s">
         <v>316</v>
       </c>
@@ -44720,7 +44723,7 @@
       </c>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A69" s="826"/>
+      <c r="A69" s="825"/>
       <c r="B69" s="75" t="s">
         <v>318</v>
       </c>
@@ -44753,7 +44756,7 @@
       </c>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A70" s="826"/>
+      <c r="A70" s="825"/>
       <c r="B70" s="370" t="s">
         <v>194</v>
       </c>
@@ -44786,7 +44789,7 @@
       </c>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A71" s="826"/>
+      <c r="A71" s="825"/>
       <c r="B71" s="370" t="s">
         <v>195</v>
       </c>
@@ -44819,7 +44822,7 @@
       </c>
     </row>
     <row r="72" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A72" s="827"/>
+      <c r="A72" s="826"/>
       <c r="B72" s="371" t="s">
         <v>196</v>
       </c>
@@ -44852,7 +44855,7 @@
       </c>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A73" s="825" t="s">
+      <c r="A73" s="824" t="s">
         <v>199</v>
       </c>
       <c r="B73" s="280" t="s">
@@ -44887,7 +44890,7 @@
       </c>
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A74" s="826"/>
+      <c r="A74" s="825"/>
       <c r="B74" s="75" t="s">
         <v>319</v>
       </c>
@@ -44920,7 +44923,7 @@
       </c>
     </row>
     <row r="75" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A75" s="827"/>
+      <c r="A75" s="826"/>
       <c r="B75" s="371" t="s">
         <v>273</v>
       </c>
@@ -44953,7 +44956,7 @@
       </c>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A76" s="825" t="s">
+      <c r="A76" s="824" t="s">
         <v>200</v>
       </c>
       <c r="B76" s="280" t="s">
@@ -44988,7 +44991,7 @@
       </c>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A77" s="826"/>
+      <c r="A77" s="825"/>
       <c r="B77" s="75" t="s">
         <v>319</v>
       </c>
@@ -45021,7 +45024,7 @@
       </c>
     </row>
     <row r="78" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A78" s="826"/>
+      <c r="A78" s="825"/>
       <c r="B78" s="370" t="s">
         <v>273</v>
       </c>
@@ -45054,7 +45057,7 @@
       </c>
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A79" s="828" t="s">
+      <c r="A79" s="818" t="s">
         <v>489</v>
       </c>
       <c r="B79" s="280" t="s">
@@ -45077,7 +45080,7 @@
       <c r="I79" s="559"/>
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A80" s="829"/>
+      <c r="A80" s="819"/>
       <c r="B80" s="75" t="s">
         <v>319</v>
       </c>
@@ -45098,7 +45101,7 @@
       <c r="I80" s="560"/>
     </row>
     <row r="81" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A81" s="830"/>
+      <c r="A81" s="820"/>
       <c r="B81" s="371" t="s">
         <v>273</v>
       </c>
@@ -45119,7 +45122,7 @@
       <c r="I81" s="576"/>
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A82" s="831" t="s">
+      <c r="A82" s="821" t="s">
         <v>490</v>
       </c>
       <c r="B82" s="280" t="s">
@@ -45142,7 +45145,7 @@
       <c r="I82" s="562"/>
     </row>
     <row r="83" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A83" s="832"/>
+      <c r="A83" s="822"/>
       <c r="B83" s="75" t="s">
         <v>319</v>
       </c>
@@ -45163,7 +45166,7 @@
       <c r="I83" s="564"/>
     </row>
     <row r="84" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A84" s="833"/>
+      <c r="A84" s="823"/>
       <c r="B84" s="371" t="s">
         <v>273</v>
       </c>
@@ -45184,7 +45187,7 @@
       <c r="I84" s="581"/>
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A85" s="828" t="s">
+      <c r="A85" s="818" t="s">
         <v>491</v>
       </c>
       <c r="B85" s="280" t="s">
@@ -45207,7 +45210,7 @@
       <c r="I85" s="580"/>
     </row>
     <row r="86" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A86" s="829"/>
+      <c r="A86" s="819"/>
       <c r="B86" s="75" t="s">
         <v>319</v>
       </c>
@@ -45228,7 +45231,7 @@
       <c r="I86" s="564"/>
     </row>
     <row r="87" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A87" s="830"/>
+      <c r="A87" s="820"/>
       <c r="B87" s="371" t="s">
         <v>273</v>
       </c>
@@ -45250,29 +45253,29 @@
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="A79:A81"/>
-    <mergeCell ref="A82:A84"/>
-    <mergeCell ref="A85:A87"/>
-    <mergeCell ref="A73:A75"/>
-    <mergeCell ref="A76:A78"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="H5:I5"/>
+    <mergeCell ref="A17:A18"/>
+    <mergeCell ref="A20:A26"/>
+    <mergeCell ref="A35:A36"/>
+    <mergeCell ref="A7:A11"/>
+    <mergeCell ref="A12:A16"/>
+    <mergeCell ref="A27:A34"/>
     <mergeCell ref="A37:A41"/>
     <mergeCell ref="A54:A63"/>
     <mergeCell ref="A64:A72"/>
     <mergeCell ref="A42:A44"/>
     <mergeCell ref="A46:A48"/>
     <mergeCell ref="A50:A52"/>
-    <mergeCell ref="A17:A18"/>
-    <mergeCell ref="A20:A26"/>
-    <mergeCell ref="A35:A36"/>
-    <mergeCell ref="A7:A11"/>
-    <mergeCell ref="A12:A16"/>
-    <mergeCell ref="A27:A34"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="F5:G5"/>
-    <mergeCell ref="H5:I5"/>
+    <mergeCell ref="A79:A81"/>
+    <mergeCell ref="A82:A84"/>
+    <mergeCell ref="A85:A87"/>
+    <mergeCell ref="A73:A75"/>
+    <mergeCell ref="A76:A78"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -45337,14 +45340,14 @@
         <v>64</v>
       </c>
       <c r="F4" s="835"/>
-      <c r="G4" s="785" t="s">
+      <c r="G4" s="775" t="s">
         <v>65</v>
       </c>
-      <c r="H4" s="786"/>
-      <c r="I4" s="785" t="s">
+      <c r="H4" s="776"/>
+      <c r="I4" s="775" t="s">
         <v>66</v>
       </c>
-      <c r="J4" s="786"/>
+      <c r="J4" s="776"/>
     </row>
     <row r="5" spans="1:10" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="550" t="s">
@@ -45352,21 +45355,21 @@
       </c>
       <c r="B5" s="550"/>
       <c r="C5" s="550"/>
-      <c r="E5" s="818" t="str">
+      <c r="E5" s="832" t="str">
         <f>Indata!D6</f>
         <v>Beslutad politik - Trafikverkets basscenario, ändras ej av EMA!</v>
       </c>
-      <c r="F5" s="819"/>
-      <c r="G5" s="818" t="str">
+      <c r="F5" s="833"/>
+      <c r="G5" s="832" t="str">
         <f>Indata!F6</f>
         <v>Policy scenario (EMA)</v>
       </c>
-      <c r="H5" s="819"/>
-      <c r="I5" s="818" t="str">
+      <c r="H5" s="833"/>
+      <c r="I5" s="832" t="str">
         <f>Indata!H6</f>
         <v>Reference scenario (EMA -beslutad politik, varierande X)</v>
       </c>
-      <c r="J5" s="819"/>
+      <c r="J5" s="833"/>
     </row>
     <row r="6" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="120" t="s">
@@ -45636,29 +45639,29 @@
     </row>
     <row r="15" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="16" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G16" s="785" t="s">
+      <c r="G16" s="775" t="s">
         <v>65</v>
       </c>
-      <c r="H16" s="786"/>
-      <c r="I16" s="785" t="s">
+      <c r="H16" s="776"/>
+      <c r="I16" s="775" t="s">
         <v>66</v>
       </c>
-      <c r="J16" s="786"/>
+      <c r="J16" s="776"/>
     </row>
     <row r="17" spans="1:10" ht="24" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A17" s="550" t="s">
         <v>476</v>
       </c>
-      <c r="G17" s="818" t="str">
+      <c r="G17" s="832" t="str">
         <f>G5</f>
         <v>Policy scenario (EMA)</v>
       </c>
-      <c r="H17" s="819"/>
-      <c r="I17" s="818" t="str">
+      <c r="H17" s="833"/>
+      <c r="I17" s="832" t="str">
         <f>I5</f>
         <v>Reference scenario (EMA -beslutad politik, varierande X)</v>
       </c>
-      <c r="J17" s="819"/>
+      <c r="J17" s="833"/>
     </row>
     <row r="18" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="G18" s="122">

</xml_diff>